<commit_message>
upgraded to Julia 1.7.3
</commit_message>
<xml_diff>
--- a/test/writer_output/Isosteric Heat Analysis.xlsx
+++ b/test/writer_output/Isosteric Heat Analysis.xlsx
@@ -598,79 +598,79 @@
         <v>293.15</v>
       </c>
       <c r="B4">
-        <v>9.119028296170422e-6</v>
+        <v>9.119028295590636e-6</v>
       </c>
       <c r="C4">
-        <v>0.018391395045482872</v>
+        <v>0.018391395045291255</v>
       </c>
       <c r="D4">
-        <v>0.03800063980479852</v>
+        <v>0.03800063980441153</v>
       </c>
       <c r="E4">
-        <v>0.05895650858192524</v>
+        <v>0.05895650858134235</v>
       </c>
       <c r="F4">
-        <v>0.08139361794483305</v>
+        <v>0.0813936179440509</v>
       </c>
       <c r="G4">
-        <v>0.10546374226553795</v>
+        <v>0.10546374226455597</v>
       </c>
       <c r="H4">
-        <v>0.13133835636167818</v>
+        <v>0.13133835636049637</v>
       </c>
       <c r="I4">
-        <v>0.15921157391688495</v>
+        <v>0.15921157391550703</v>
       </c>
       <c r="J4">
-        <v>0.18930353366924638</v>
+        <v>0.18930353366767502</v>
       </c>
       <c r="K4">
-        <v>0.2218642845351649</v>
+        <v>0.2218642845334078</v>
       </c>
       <c r="L4">
-        <v>0.2571782145127691</v>
+        <v>0.2571782145108355</v>
       </c>
       <c r="M4">
-        <v>0.29556905287542284</v>
+        <v>0.2955690528733275</v>
       </c>
       <c r="N4">
-        <v>0.33740544571569475</v>
+        <v>0.3374054457134568</v>
       </c>
       <c r="O4">
-        <v>0.3831070541686949</v>
+        <v>0.3831070541663378</v>
       </c>
       <c r="P4">
-        <v>0.43315104303962343</v>
+        <v>0.43315104303717805</v>
       </c>
       <c r="Q4">
-        <v>0.488078703082626</v>
+        <v>0.48807870308013246</v>
       </c>
       <c r="R4">
-        <v>0.5485017693817901</v>
+        <v>0.5485017693792951</v>
       </c>
       <c r="S4">
-        <v>0.615107749153492</v>
+        <v>0.6151077491510532</v>
       </c>
       <c r="T4">
-        <v>0.68866325041921</v>
+        <v>0.6886632504168949</v>
       </c>
       <c r="U4">
-        <v>0.7700139227090961</v>
+        <v>0.7700139227069838</v>
       </c>
       <c r="V4">
-        <v>0.8600792321815738</v>
+        <v>0.86007923217975</v>
       </c>
       <c r="W4">
-        <v>0.9598400023437031</v>
+        <v>0.9598400023422629</v>
       </c>
       <c r="X4">
-        <v>1.070316635349533</v>
+        <v>1.070316635348572</v>
       </c>
       <c r="Y4">
-        <v>1.1925364269474923</v>
+        <v>1.1925364269471013</v>
       </c>
       <c r="Z4">
-        <v>1.3274896392376172</v>
+        <v>1.3274896392378743</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -678,79 +678,79 @@
         <v>300.15</v>
       </c>
       <c r="B5">
-        <v>1.0965195990091104e-5</v>
+        <v>1.0965195991384605e-5</v>
       </c>
       <c r="C5">
-        <v>0.022131436836201182</v>
+        <v>0.022131436836561016</v>
       </c>
       <c r="D5">
-        <v>0.045766170670456886</v>
+        <v>0.045766170671152864</v>
       </c>
       <c r="E5">
-        <v>0.07106892993093257</v>
+        <v>0.07106892993193813</v>
       </c>
       <c r="F5">
-        <v>0.09821389842341031</v>
+        <v>0.09821389842468753</v>
       </c>
       <c r="G5">
-        <v>0.12739896036981394</v>
+        <v>0.1273989603713198</v>
       </c>
       <c r="H5">
-        <v>0.1588495766923801</v>
+        <v>0.15884957669406077</v>
       </c>
       <c r="I5">
-        <v>0.1928233708826446</v>
+        <v>0.19282337088443346</v>
       </c>
       <c r="J5">
-        <v>0.22961555629574612</v>
+        <v>0.22961555629756145</v>
       </c>
       <c r="K5">
-        <v>0.269565355834171</v>
+        <v>0.2695653558359179</v>
       </c>
       <c r="L5">
-        <v>0.31306358231659664</v>
+        <v>0.3130635823181577</v>
       </c>
       <c r="M5">
-        <v>0.3605615593032984</v>
+        <v>0.36056155930453454</v>
       </c>
       <c r="N5">
-        <v>0.41258156074680385</v>
+        <v>0.4125815607475511</v>
       </c>
       <c r="O5">
-        <v>0.46972892193805754</v>
+        <v>0.469728921938125</v>
       </c>
       <c r="P5">
-        <v>0.532705905343227</v>
+        <v>0.5327059053423923</v>
       </c>
       <c r="Q5">
-        <v>0.6023272648613003</v>
+        <v>0.6023272648593121</v>
       </c>
       <c r="R5">
-        <v>0.679537199821544</v>
+        <v>0.6795371998181226</v>
       </c>
       <c r="S5">
-        <v>0.7654269702565001</v>
+        <v>0.7654269702513454</v>
       </c>
       <c r="T5">
-        <v>0.8612517906350058</v>
+        <v>0.8612517906278102</v>
       </c>
       <c r="U5">
-        <v>0.9684446658464305</v>
+        <v>0.9684446658369041</v>
       </c>
       <c r="V5">
-        <v>1.088623554900231</v>
+        <v>1.0886235548881442</v>
       </c>
       <c r="W5">
-        <v>1.2235867286315227</v>
+        <v>1.2235867286167659</v>
       </c>
       <c r="X5">
-        <v>1.3752897350451516</v>
+        <v>1.3752897350278257</v>
       </c>
       <c r="Y5">
-        <v>1.5457966608784894</v>
+        <v>1.545796660859025</v>
       </c>
       <c r="Z5">
-        <v>1.7371994464902663</v>
+        <v>1.7371994464695681</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -758,79 +758,79 @@
         <v>308.15</v>
       </c>
       <c r="B6">
-        <v>1.2890321023727155e-5</v>
+        <v>1.2890321023558026e-5</v>
       </c>
       <c r="C6">
-        <v>0.026157627651847887</v>
+        <v>0.02615762765182807</v>
       </c>
       <c r="D6">
-        <v>0.054401479686169055</v>
+        <v>0.05440147968612817</v>
       </c>
       <c r="E6">
-        <v>0.08499016592290676</v>
+        <v>0.08499016592284361</v>
       </c>
       <c r="F6">
-        <v>0.1182060402362688</v>
+        <v>0.11820604023617899</v>
       </c>
       <c r="G6">
-        <v>0.15437439687535437</v>
+        <v>0.15437439687523324</v>
       </c>
       <c r="H6">
-        <v>0.19387088891352675</v>
+        <v>0.19387088891337295</v>
       </c>
       <c r="I6">
-        <v>0.23713020560857104</v>
+        <v>0.23713020560837955</v>
       </c>
       <c r="J6">
-        <v>0.2846561325326306</v>
+        <v>0.2846561325323957</v>
       </c>
       <c r="K6">
-        <v>0.33703305949405277</v>
+        <v>0.3370330594937694</v>
       </c>
       <c r="L6">
-        <v>0.39493888258541165</v>
+        <v>0.394938882585073</v>
       </c>
       <c r="M6">
-        <v>0.459159033973199</v>
+        <v>0.4591590339727979</v>
       </c>
       <c r="N6">
-        <v>0.5306010202317961</v>
+        <v>0.530601020231325</v>
       </c>
       <c r="O6">
-        <v>0.6103083018201666</v>
+        <v>0.6103083018196175</v>
       </c>
       <c r="P6">
-        <v>0.6994715503091371</v>
+        <v>0.6994715503085004</v>
       </c>
       <c r="Q6">
-        <v>0.7994342572943302</v>
+        <v>0.7994342572935972</v>
       </c>
       <c r="R6">
-        <v>0.9116884141735291</v>
+        <v>0.9116884141726913</v>
       </c>
       <c r="S6">
-        <v>1.037854797426806</v>
+        <v>1.0378547974258567</v>
       </c>
       <c r="T6">
-        <v>1.1796418361825063</v>
+        <v>1.1796418361814414</v>
       </c>
       <c r="U6">
-        <v>1.3387779949868457</v>
+        <v>1.338777994985664</v>
       </c>
       <c r="V6">
-        <v>1.5169160975954334</v>
+        <v>1.516916097594143</v>
       </c>
       <c r="W6">
-        <v>1.7155146036246816</v>
+        <v>1.715514603623294</v>
       </c>
       <c r="X6">
-        <v>1.935709665603194</v>
+        <v>1.9357096656017325</v>
       </c>
       <c r="Y6">
-        <v>2.1781998613292473</v>
+        <v>2.1781998613277422</v>
       </c>
       <c r="Z6">
-        <v>2.443168373187182</v>
+        <v>2.4431683731856744</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -838,79 +838,79 @@
         <v>323.15</v>
       </c>
       <c r="B7">
-        <v>1.8473750063392738e-5</v>
+        <v>1.8473750063586352e-5</v>
       </c>
       <c r="C7">
-        <v>0.03742548090100247</v>
+        <v>0.03742548090073113</v>
       </c>
       <c r="D7">
-        <v>0.07769610638778919</v>
+        <v>0.07769610638724225</v>
       </c>
       <c r="E7">
-        <v>0.12114688103380995</v>
+        <v>0.12114688103298468</v>
       </c>
       <c r="F7">
-        <v>0.16813832487272748</v>
+        <v>0.16813832487161998</v>
       </c>
       <c r="G7">
-        <v>0.21908185899382918</v>
+        <v>0.21908185899244062</v>
       </c>
       <c r="H7">
-        <v>0.27444777774580387</v>
+        <v>0.2744477777441387</v>
       </c>
       <c r="I7">
-        <v>0.33477437348934974</v>
+        <v>0.33477437348741135</v>
       </c>
       <c r="J7">
-        <v>0.4006782641287994</v>
+        <v>0.4006782641265966</v>
       </c>
       <c r="K7">
-        <v>0.4728658937146207</v>
+        <v>0.472865893712167</v>
       </c>
       <c r="L7">
-        <v>0.5521460388223153</v>
+        <v>0.5521460388196261</v>
       </c>
       <c r="M7">
-        <v>0.639442932047627</v>
+        <v>0.6394429320447246</v>
       </c>
       <c r="N7">
-        <v>0.7358092770039117</v>
+        <v>0.7358092770008248</v>
       </c>
       <c r="O7">
-        <v>0.8424379435924141</v>
+        <v>0.8424379435891721</v>
       </c>
       <c r="P7">
-        <v>0.9606704751589408</v>
+        <v>0.960670475155582</v>
       </c>
       <c r="Q7">
-        <v>1.0919997208629306</v>
+        <v>1.0919997208594912</v>
       </c>
       <c r="R7">
-        <v>1.2380630097120604</v>
+        <v>1.2380630097085752</v>
       </c>
       <c r="S7">
-        <v>1.400621515003608</v>
+        <v>1.400621515000105</v>
       </c>
       <c r="T7">
-        <v>1.5815212024126364</v>
+        <v>1.5815212024091216</v>
       </c>
       <c r="U7">
-        <v>1.7826315713529446</v>
+        <v>1.7826315713493963</v>
       </c>
       <c r="V7">
-        <v>2.005760899003269</v>
+        <v>2.0057608989996214</v>
       </c>
       <c r="W7">
-        <v>2.2525512184209866</v>
+        <v>2.2525512184171097</v>
       </c>
       <c r="X7">
-        <v>2.524362379079606</v>
+        <v>2.5243623790752947</v>
       </c>
       <c r="Y7">
-        <v>2.8221606553925147</v>
+        <v>2.8221606553874725</v>
       </c>
       <c r="Z7">
-        <v>3.1464308987103604</v>
+        <v>3.1464308987041987</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -1083,79 +1083,79 @@
         <v>0.003411222923418046</v>
       </c>
       <c r="B12">
-        <v>-11.605147306027055</v>
+        <v>-11.605147306090634</v>
       </c>
       <c r="C12">
-        <v>-3.995872384326091</v>
+        <v>-3.9958723843365096</v>
       </c>
       <c r="D12">
-        <v>-3.2701522824291094</v>
+        <v>-3.2701522824392932</v>
       </c>
       <c r="E12">
-        <v>-2.8309552495789054</v>
+        <v>-2.830955249588792</v>
       </c>
       <c r="F12">
-        <v>-2.5084584126734972</v>
+        <v>-2.5084584126831064</v>
       </c>
       <c r="G12">
-        <v>-2.2493880603440455</v>
+        <v>-2.2493880603533567</v>
       </c>
       <c r="H12">
-        <v>-2.029978412674971</v>
+        <v>-2.029978412683969</v>
       </c>
       <c r="I12">
-        <v>-1.8375213077314607</v>
+        <v>-1.8375213077401154</v>
       </c>
       <c r="J12">
-        <v>-1.6644035539086177</v>
+        <v>-1.6644035539169184</v>
       </c>
       <c r="K12">
-        <v>-1.5056894149714783</v>
+        <v>-1.505689414979398</v>
       </c>
       <c r="L12">
-        <v>-1.3579859927225832</v>
+        <v>-1.357985992730102</v>
       </c>
       <c r="M12">
-        <v>-1.2188527879617348</v>
+        <v>-1.2188527879688238</v>
       </c>
       <c r="N12">
-        <v>-1.0864699687643187</v>
+        <v>-1.0864699687709516</v>
       </c>
       <c r="O12">
-        <v>-0.9594408140577052</v>
+        <v>-0.9594408140638578</v>
       </c>
       <c r="P12">
-        <v>-0.8366687826155881</v>
+        <v>-0.8366687826212337</v>
       </c>
       <c r="Q12">
-        <v>-0.7172786093240364</v>
+        <v>-0.7172786093291453</v>
       </c>
       <c r="R12">
-        <v>-0.6005647734164671</v>
+        <v>-0.6005647734210159</v>
       </c>
       <c r="S12">
-        <v>-0.4859578246460787</v>
+        <v>-0.48595782465004356</v>
       </c>
       <c r="T12">
-        <v>-0.37300287865207166</v>
+        <v>-0.3730028786554333</v>
       </c>
       <c r="U12">
-        <v>-0.2613466828574903</v>
+        <v>-0.2613466828602335</v>
       </c>
       <c r="V12">
-        <v>-0.15073076353464188</v>
+        <v>-0.15073076353676232</v>
       </c>
       <c r="W12">
-        <v>-0.04098867263558969</v>
+        <v>-0.04098867263709024</v>
       </c>
       <c r="X12">
-        <v>0.06795452558527898</v>
+        <v>0.0679545255843811</v>
       </c>
       <c r="Y12">
-        <v>0.17608249002031057</v>
+        <v>0.1760824900199827</v>
       </c>
       <c r="Z12">
-        <v>0.28328966938607403</v>
+        <v>0.28328966938626776</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -1163,79 +1163,79 @@
         <v>0.003331667499583542</v>
       </c>
       <c r="B13">
-        <v>-11.420784302100849</v>
+        <v>-11.420784301982884</v>
       </c>
       <c r="C13">
-        <v>-3.81075619995043</v>
+        <v>-3.810756199934171</v>
       </c>
       <c r="D13">
-        <v>-3.084210092434169</v>
+        <v>-3.0842100924189615</v>
       </c>
       <c r="E13">
-        <v>-2.6441050288075134</v>
+        <v>-2.6441050287933643</v>
       </c>
       <c r="F13">
-        <v>-2.3206075418297756</v>
+        <v>-2.3206075418167713</v>
       </c>
       <c r="G13">
-        <v>-2.060431696239898</v>
+        <v>-2.0604316962280778</v>
       </c>
       <c r="H13">
-        <v>-1.8397975830962243</v>
+        <v>-1.839797583085644</v>
       </c>
       <c r="I13">
-        <v>-1.6459806858810546</v>
+        <v>-1.6459806858717774</v>
       </c>
       <c r="J13">
-        <v>-1.4713488629305844</v>
+        <v>-1.4713488629226783</v>
       </c>
       <c r="K13">
-        <v>-1.3109444102998593</v>
+        <v>-1.310944410293379</v>
       </c>
       <c r="L13">
-        <v>-1.1613489706801106</v>
+        <v>-1.1613489706751243</v>
       </c>
       <c r="M13">
-        <v>-1.0200925759383102</v>
+        <v>-1.0200925759348818</v>
       </c>
       <c r="N13">
-        <v>-0.8853213697294672</v>
+        <v>-0.8853213697276561</v>
       </c>
       <c r="O13">
-        <v>-0.7555995125030412</v>
+        <v>-0.7555995125028976</v>
       </c>
       <c r="P13">
-        <v>-0.6297857794378303</v>
+        <v>-0.6297857794393974</v>
       </c>
       <c r="Q13">
-        <v>-0.5069543520485047</v>
+        <v>-0.5069543520518055</v>
       </c>
       <c r="R13">
-        <v>-0.38634330101520237</v>
+        <v>-0.38634330102023734</v>
       </c>
       <c r="S13">
-        <v>-0.2673214697985593</v>
+        <v>-0.2673214698052937</v>
       </c>
       <c r="T13">
-        <v>-0.1493683775446672</v>
+        <v>-0.14936837755302199</v>
       </c>
       <c r="U13">
-        <v>-0.03206393163777815</v>
+        <v>-0.03206393164761493</v>
       </c>
       <c r="V13">
-        <v>0.08491410457574017</v>
+        <v>0.08491410456463735</v>
       </c>
       <c r="W13">
-        <v>0.20178648706998767</v>
+        <v>0.20178648705792734</v>
       </c>
       <c r="X13">
-        <v>0.31866442531742684</v>
+        <v>0.31866442530482886</v>
       </c>
       <c r="Y13">
-        <v>0.43553941556311576</v>
+        <v>0.4355394155505239</v>
       </c>
       <c r="Z13">
-        <v>0.5522743030567119</v>
+        <v>0.5522743030447973</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -1243,79 +1243,79 @@
         <v>0.0032451728054518907</v>
       </c>
       <c r="B14">
-        <v>-11.259033836456956</v>
+        <v>-11.259033836470078</v>
       </c>
       <c r="C14">
-        <v>-3.643614442596813</v>
+        <v>-3.6436144425975705</v>
       </c>
       <c r="D14">
-        <v>-2.911363925376755</v>
+        <v>-2.9113639253775063</v>
       </c>
       <c r="E14">
-        <v>-2.4652197242096325</v>
+        <v>-2.4652197242103755</v>
       </c>
       <c r="F14">
-        <v>-2.135326073486108</v>
+        <v>-2.1353260734868678</v>
       </c>
       <c r="G14">
-        <v>-1.868374478487823</v>
+        <v>-1.8683744784886074</v>
       </c>
       <c r="H14">
-        <v>-1.6405628625405537</v>
+        <v>-1.640562862541347</v>
       </c>
       <c r="I14">
-        <v>-1.43914589795339</v>
+        <v>-1.4391458979541976</v>
       </c>
       <c r="J14">
-        <v>-1.2564733797010779</v>
+        <v>-1.2564733797019032</v>
       </c>
       <c r="K14">
-        <v>-1.087574254052325</v>
+        <v>-1.0875742540531659</v>
       </c>
       <c r="L14">
-        <v>-0.9290242536844393</v>
+        <v>-0.9290242536852968</v>
       </c>
       <c r="M14">
-        <v>-0.7783586496872219</v>
+        <v>-0.7783586496880955</v>
       </c>
       <c r="N14">
-        <v>-0.6337449144914354</v>
+        <v>-0.6337449144923233</v>
       </c>
       <c r="O14">
-        <v>-0.4937910366728759</v>
+        <v>-0.4937910366737756</v>
       </c>
       <c r="P14">
-        <v>-0.35743015717027365</v>
+        <v>-0.357430157171184</v>
       </c>
       <c r="Q14">
-        <v>-0.22385097986487862</v>
+        <v>-0.22385097986579547</v>
       </c>
       <c r="R14">
-        <v>-0.09245699840936435</v>
+        <v>-0.09245699841028326</v>
       </c>
       <c r="S14">
-        <v>0.03715588808655996</v>
+        <v>0.03715588808564534</v>
       </c>
       <c r="T14">
-        <v>0.1652108637445336</v>
+        <v>0.16521086374363084</v>
       </c>
       <c r="U14">
-        <v>0.2917572538492102</v>
+        <v>0.2917572538483275</v>
       </c>
       <c r="V14">
-        <v>0.41667939072572685</v>
+        <v>0.4166793907248761</v>
       </c>
       <c r="W14">
-        <v>0.5397130960313329</v>
+        <v>0.5397130960305241</v>
       </c>
       <c r="X14">
-        <v>0.6604740114942905</v>
+        <v>0.6604740114935356</v>
       </c>
       <c r="Y14">
-        <v>0.7784987839964441</v>
+        <v>0.7784987839957532</v>
       </c>
       <c r="Z14">
-        <v>0.8932957105667424</v>
+        <v>0.8932957105661253</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -1323,79 +1323,79 @@
         <v>0.0030945381401825778</v>
       </c>
       <c r="B15">
-        <v>-10.899159748986126</v>
+        <v>-10.899159748975645</v>
       </c>
       <c r="C15">
-        <v>-3.285403499032817</v>
+        <v>-3.285403499040067</v>
       </c>
       <c r="D15">
-        <v>-2.5549501337033895</v>
+        <v>-2.554950133710429</v>
       </c>
       <c r="E15">
-        <v>-2.110751576716211</v>
+        <v>-2.1107515767230227</v>
       </c>
       <c r="F15">
-        <v>-1.7829682760180394</v>
+        <v>-1.7829682760246264</v>
       </c>
       <c r="G15">
-        <v>-1.5183098336460303</v>
+        <v>-1.5183098336523684</v>
       </c>
       <c r="H15">
-        <v>-1.2929942811376074</v>
+        <v>-1.2929942811436748</v>
       </c>
       <c r="I15">
-        <v>-1.0942984860402398</v>
+        <v>-1.09429848604603</v>
       </c>
       <c r="J15">
-        <v>-0.9145965075610273</v>
+        <v>-0.9145965075665251</v>
       </c>
       <c r="K15">
-        <v>-0.7489434534924628</v>
+        <v>-0.7489434534976518</v>
       </c>
       <c r="L15">
-        <v>-0.5939427046117786</v>
+        <v>-0.593942704616649</v>
       </c>
       <c r="M15">
-        <v>-0.44715790033829933</v>
+        <v>-0.44715790034283837</v>
       </c>
       <c r="N15">
-        <v>-0.306784328339963</v>
+        <v>-0.3067843283441583</v>
       </c>
       <c r="O15">
-        <v>-0.17145527692553925</v>
+        <v>-0.17145527692938756</v>
       </c>
       <c r="P15">
-        <v>-0.04012382667225934</v>
+        <v>-0.040123826675755606</v>
       </c>
       <c r="Q15">
-        <v>0.08801062170265372</v>
+        <v>0.08801062169950402</v>
       </c>
       <c r="R15">
-        <v>0.21354806934207468</v>
+        <v>0.21354806933925963</v>
       </c>
       <c r="S15">
-        <v>0.33691607739761303</v>
+        <v>0.33691607739511187</v>
       </c>
       <c r="T15">
-        <v>0.4583871701944943</v>
+        <v>0.45838717019227193</v>
       </c>
       <c r="U15">
-        <v>0.5780906834030081</v>
+        <v>0.5780906834010175</v>
       </c>
       <c r="V15">
-        <v>0.6960234895160966</v>
+        <v>0.696023489514278</v>
       </c>
       <c r="W15">
-        <v>0.8120634487195262</v>
+        <v>0.812063448717805</v>
       </c>
       <c r="X15">
-        <v>0.9259885077011974</v>
+        <v>0.9259885076994896</v>
       </c>
       <c r="Y15">
-        <v>1.0375027814319202</v>
+        <v>1.0375027814301336</v>
       </c>
       <c r="Z15">
-        <v>1.1462687624248866</v>
+        <v>1.1462687624229284</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -1419,10 +1419,10 @@
         <v>0.001</v>
       </c>
       <c r="B19">
-        <v>-18769.788628103597</v>
+        <v>-18769.7886287209</v>
       </c>
       <c r="C19">
-        <v>28.916526722709897</v>
+        <v>28.9165267824289</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -1430,10 +1430,10 @@
         <v>1.9535148291666666</v>
       </c>
       <c r="B20">
-        <v>-18842.17654001701</v>
+        <v>-18842.176539940716</v>
       </c>
       <c r="C20">
-        <v>24.895705987396653</v>
+        <v>24.895705999519482</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -1441,10 +1441,10 @@
         <v>3.906029658333333</v>
       </c>
       <c r="B21">
-        <v>-18918.36311340451</v>
+        <v>-18918.363113306656</v>
       </c>
       <c r="C21">
-        <v>20.5324858584102</v>
+        <v>20.532485868655208</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -1452,10 +1452,10 @@
         <v>5.8585444875</v>
       </c>
       <c r="B22">
-        <v>-18998.600511017383</v>
+        <v>-18998.60051089893</v>
       </c>
       <c r="C22">
-        <v>15.798301322098341</v>
+        <v>15.79830133055239</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -1463,10 +1463,10 @@
         <v>7.811059316666666</v>
       </c>
       <c r="B23">
-        <v>-19083.14849344413</v>
+        <v>-19083.14849330155</v>
       </c>
       <c r="C23">
-        <v>10.694831742301293</v>
+        <v>10.694831749365973</v>
       </c>
     </row>
     <row r="24" spans="1:26">
@@ -1474,10 +1474,10 @@
         <v>9.763574145833333</v>
       </c>
       <c r="B24">
-        <v>-19172.267917768964</v>
+        <v>-19172.26791759342</v>
       </c>
       <c r="C24">
-        <v>5.459245857298383</v>
+        <v>5.459245865137787</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -1485,10 +1485,10 @@
         <v>11.716088975</v>
       </c>
       <c r="B25">
-        <v>-19266.210303255364</v>
+        <v>-19266.21030305189</v>
       </c>
       <c r="C25">
-        <v>3.7329966272703228</v>
+        <v>3.7329966388079896</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -1496,10 +1496,10 @@
         <v>13.668603804166668</v>
       </c>
       <c r="B26">
-        <v>-19365.201720085297</v>
+        <v>-19365.20171985812</v>
       </c>
       <c r="C26">
-        <v>9.503422450378403</v>
+        <v>9.50342245952136</v>
       </c>
     </row>
     <row r="27" spans="1:26">
@@ -1507,10 +1507,10 @@
         <v>15.621118633333333</v>
       </c>
       <c r="B27">
-        <v>-19469.41863788263</v>
+        <v>-19469.418637618724</v>
       </c>
       <c r="C27">
-        <v>17.01390500689444</v>
+        <v>17.013905017925232</v>
       </c>
     </row>
     <row r="28" spans="1:26">
@@ -1518,10 +1518,10 @@
         <v>17.5736334625</v>
       </c>
       <c r="B28">
-        <v>-19578.952628465584</v>
+        <v>-19578.9526281772</v>
       </c>
       <c r="C28">
-        <v>25.51045023931199</v>
+        <v>25.510450253530045</v>
       </c>
     </row>
     <row r="29" spans="1:26">
@@ -1529,10 +1529,10 @@
         <v>19.52614829166667</v>
       </c>
       <c r="B29">
-        <v>-19693.76002113267</v>
+        <v>-19693.760020796435</v>
       </c>
       <c r="C29">
-        <v>34.99463568741852</v>
+        <v>34.99463570551486</v>
       </c>
     </row>
     <row r="30" spans="1:26">
@@ -1540,10 +1540,10 @@
         <v>21.478663120833332</v>
       </c>
       <c r="B30">
-        <v>-19813.591930455947</v>
+        <v>-19813.59193008914</v>
       </c>
       <c r="C30">
-        <v>45.54937971763629</v>
+        <v>45.54937974020265</v>
       </c>
     </row>
     <row r="31" spans="1:26">
@@ -1551,10 +1551,10 @@
         <v>23.43117795</v>
       </c>
       <c r="B31">
-        <v>-19937.89987139893</v>
+        <v>-19937.899870973073</v>
       </c>
       <c r="C31">
-        <v>57.276264873249545</v>
+        <v>57.27626490079205</v>
       </c>
     </row>
     <row r="32" spans="1:26">
@@ -1562,10 +1562,10 @@
         <v>25.383692779166665</v>
       </c>
       <c r="B32">
-        <v>-20065.713072881823</v>
+        <v>-20065.71307241521</v>
       </c>
       <c r="C32">
-        <v>70.27744434638686</v>
+        <v>70.27744437948374</v>
       </c>
     </row>
     <row r="33" spans="1:26">
@@ -1573,10 +1573,10 @@
         <v>27.336207608333336</v>
       </c>
       <c r="B33">
-        <v>-20195.486594613427</v>
+        <v>-20195.4865940917</v>
       </c>
       <c r="C33">
-        <v>84.64185725038128</v>
+        <v>84.64185728956016</v>
       </c>
     </row>
     <row r="34" spans="1:26">
@@ -1584,10 +1584,10 @@
         <v>29.2887224375</v>
       </c>
       <c r="B34">
-        <v>-20324.925793058475</v>
+        <v>-20324.925792473714</v>
       </c>
       <c r="C34">
-        <v>100.4288258025177</v>
+        <v>100.42882584829684</v>
       </c>
     </row>
     <row r="35" spans="1:26">
@@ -1595,10 +1595,10 @@
         <v>31.241237266666666</v>
       </c>
       <c r="B35">
-        <v>-20450.80402198295</v>
+        <v>-20450.804021332104</v>
       </c>
       <c r="C35">
-        <v>117.64706295353814</v>
+        <v>117.6470630063938</v>
       </c>
     </row>
     <row r="36" spans="1:26">
@@ -1606,10 +1606,10 @@
         <v>33.19375209583334</v>
       </c>
       <c r="B36">
-        <v>-20568.807455089296</v>
+        <v>-20568.807454374753</v>
       </c>
       <c r="C36">
-        <v>136.22899345947945</v>
+        <v>136.22899351979768</v>
       </c>
     </row>
     <row r="37" spans="1:26">
@@ -1617,10 +1617,10 @@
         <v>35.146266925</v>
       </c>
       <c r="B37">
-        <v>-20673.462135937447</v>
+        <v>-20673.46213514969</v>
       </c>
       <c r="C37">
-        <v>156.00225398128475</v>
+        <v>156.00225404923268</v>
       </c>
     </row>
     <row r="38" spans="1:26">
@@ -1628,10 +1628,10 @@
         <v>37.098781754166666</v>
       </c>
       <c r="B38">
-        <v>-20758.217943400083</v>
+        <v>-20758.217942523377</v>
       </c>
       <c r="C38">
-        <v>176.66288781630269</v>
+        <v>176.66288789174283</v>
       </c>
     </row>
     <row r="39" spans="1:26">
@@ -1639,10 +1639,10 @@
         <v>39.05129658333333</v>
       </c>
       <c r="B39">
-        <v>-20815.77009874279</v>
+        <v>-20815.770097776793</v>
       </c>
       <c r="C39">
-        <v>197.75783145550056</v>
+        <v>197.75783153799966</v>
       </c>
     </row>
     <row r="40" spans="1:26">
@@ -1650,10 +1650,10 @@
         <v>41.0038114125</v>
       </c>
       <c r="B40">
-        <v>-20838.674217523116</v>
+        <v>-20838.674216468622</v>
       </c>
       <c r="C40">
-        <v>218.68668534132516</v>
+        <v>218.68668543002858</v>
       </c>
     </row>
     <row r="41" spans="1:26">
@@ -1661,10 +1661,10 @@
         <v>42.956326241666666</v>
       </c>
       <c r="B41">
-        <v>-20820.241633788064</v>
+        <v>-20820.241632622</v>
       </c>
       <c r="C41">
-        <v>238.7325051409998</v>
+        <v>238.73250523449457</v>
       </c>
     </row>
     <row r="42" spans="1:26">
@@ -1672,10 +1672,10 @@
         <v>44.90884107083333</v>
       </c>
       <c r="B42">
-        <v>-20755.591493157914</v>
+        <v>-20755.591491882704</v>
       </c>
       <c r="C42">
-        <v>257.12635448665884</v>
+        <v>257.1263545832731</v>
       </c>
     </row>
     <row r="43" spans="1:26">
@@ -1683,10 +1683,10 @@
         <v>46.8613559</v>
       </c>
       <c r="B43">
-        <v>-20642.62100251357</v>
+        <v>-20642.621001125444</v>
       </c>
       <c r="C43">
-        <v>273.1401170699936</v>
+        <v>273.14011716776565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed model uncertainty from isosteric heats and new version
</commit_message>
<xml_diff>
--- a/test/writer_output/Isosteric Heat Analysis.xlsx
+++ b/test/writer_output/Isosteric Heat Analysis.xlsx
@@ -1419,10 +1419,10 @@
         <v>0.001</v>
       </c>
       <c r="B19">
-        <v>-18769.7886287209</v>
+        <v>-18378.575811054645</v>
       </c>
       <c r="C19">
-        <v>28.9165267824289</v>
+        <v>579.5134118970051</v>
       </c>
     </row>
     <row r="20" spans="1:26">
@@ -1430,10 +1430,10 @@
         <v>1.9535148291666666</v>
       </c>
       <c r="B20">
-        <v>-18842.176539940716</v>
+        <v>-18514.235348989187</v>
       </c>
       <c r="C20">
-        <v>24.895705999519482</v>
+        <v>496.3133064403586</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -1441,10 +1441,10 @@
         <v>3.906029658333333</v>
       </c>
       <c r="B21">
-        <v>-18918.363113306656</v>
+        <v>-18657.396694491377</v>
       </c>
       <c r="C21">
-        <v>20.532485868655208</v>
+        <v>408.4859772109164</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -1452,10 +1452,10 @@
         <v>5.8585444875</v>
       </c>
       <c r="B22">
-        <v>-18998.60051089893</v>
+        <v>-18808.52702744859</v>
       </c>
       <c r="C22">
-        <v>15.79830133055239</v>
+        <v>316.3657643973871</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -1463,10 +1463,10 @@
         <v>7.811059316666666</v>
       </c>
       <c r="B23">
-        <v>-19083.14849330155</v>
+        <v>-18968.09808708953</v>
       </c>
       <c r="C23">
-        <v>10.694831749365973</v>
+        <v>221.76317533168935</v>
       </c>
     </row>
     <row r="24" spans="1:26">
@@ -1474,10 +1474,10 @@
         <v>9.763574145833333</v>
       </c>
       <c r="B24">
-        <v>-19172.26791759342</v>
+        <v>-19136.574085987635</v>
       </c>
       <c r="C24">
-        <v>5.459245865137787</v>
+        <v>133.8686923887531</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -1485,10 +1485,10 @@
         <v>11.716088975</v>
       </c>
       <c r="B25">
-        <v>-19266.21030305189</v>
+        <v>-19314.394300115335</v>
       </c>
       <c r="C25">
-        <v>3.7329966388079896</v>
+        <v>103.9677643832511</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -1496,10 +1496,10 @@
         <v>13.668603804166668</v>
       </c>
       <c r="B26">
-        <v>-19365.20171985812</v>
+        <v>-19501.94852921517</v>
       </c>
       <c r="C26">
-        <v>9.50342245952136</v>
+        <v>182.0824505092694</v>
       </c>
     </row>
     <row r="27" spans="1:26">
@@ -1507,10 +1507,10 @@
         <v>15.621118633333333</v>
       </c>
       <c r="B27">
-        <v>-19469.418637618724</v>
+        <v>-19699.543131485745</v>
       </c>
       <c r="C27">
-        <v>17.013905017925232</v>
+        <v>301.9546068240059</v>
       </c>
     </row>
     <row r="28" spans="1:26">
@@ -1518,10 +1518,10 @@
         <v>17.5736334625</v>
       </c>
       <c r="B28">
-        <v>-19578.9526281772</v>
+        <v>-19907.35478495998</v>
       </c>
       <c r="C28">
-        <v>25.510450253530045</v>
+        <v>438.28138925260197</v>
       </c>
     </row>
     <row r="29" spans="1:26">
@@ -1529,10 +1529,10 @@
         <v>19.52614829166667</v>
       </c>
       <c r="B29">
-        <v>-19693.760020796435</v>
+        <v>-20125.368576439698</v>
       </c>
       <c r="C29">
-        <v>34.99463570551486</v>
+        <v>586.6344217497052</v>
       </c>
     </row>
     <row r="30" spans="1:26">
@@ -1540,10 +1540,10 @@
         <v>21.478663120833332</v>
       </c>
       <c r="B30">
-        <v>-19813.59193008914</v>
+        <v>-20353.296595534208</v>
       </c>
       <c r="C30">
-        <v>45.54937974020265</v>
+        <v>746.0290239942018</v>
       </c>
     </row>
     <row r="31" spans="1:26">
@@ -1551,10 +1551,10 @@
         <v>23.43117795</v>
       </c>
       <c r="B31">
-        <v>-19937.899870973073</v>
+        <v>-20590.473158177017</v>
       </c>
       <c r="C31">
-        <v>57.27626490079205</v>
+        <v>916.1892658911182</v>
       </c>
     </row>
     <row r="32" spans="1:26">
@@ -1562,10 +1562,10 @@
         <v>25.383692779166665</v>
       </c>
       <c r="B32">
-        <v>-20065.71307241521</v>
+        <v>-20835.72351462588</v>
       </c>
       <c r="C32">
-        <v>70.27744437948374</v>
+        <v>1096.8900903129013</v>
       </c>
     </row>
     <row r="33" spans="1:26">
@@ -1573,10 +1573,10 @@
         <v>27.336207608333336</v>
       </c>
       <c r="B33">
-        <v>-20195.4865940917</v>
+        <v>-21087.20505578697</v>
       </c>
       <c r="C33">
-        <v>84.64185728956016</v>
+        <v>1287.6808536999324</v>
       </c>
     </row>
     <row r="34" spans="1:26">
@@ -1584,10 +1584,10 @@
         <v>29.2887224375</v>
       </c>
       <c r="B34">
-        <v>-20324.925792473714</v>
+        <v>-21342.224515142654</v>
       </c>
       <c r="C34">
-        <v>100.42882584829684</v>
+        <v>1487.6929961186208</v>
       </c>
     </row>
     <row r="35" spans="1:26">
@@ -1595,10 +1595,10 @@
         <v>31.241237266666666</v>
       </c>
       <c r="B35">
-        <v>-20450.804021332104</v>
+        <v>-21597.042519167004</v>
       </c>
       <c r="C35">
-        <v>117.6470630063938</v>
+        <v>1695.466412031768</v>
       </c>
     </row>
     <row r="36" spans="1:26">
@@ -1606,10 +1606,10 @@
         <v>33.19375209583334</v>
       </c>
       <c r="B36">
-        <v>-20568.807454374753</v>
+        <v>-21846.688900679317</v>
       </c>
       <c r="C36">
-        <v>136.22899351979768</v>
+        <v>1908.790186204067</v>
       </c>
     </row>
     <row r="37" spans="1:26">
@@ -1617,10 +1617,10 @@
         <v>35.146266925</v>
       </c>
       <c r="B37">
-        <v>-20673.46213514969</v>
+        <v>-22084.828273975676</v>
       </c>
       <c r="C37">
-        <v>156.00225404923268</v>
+        <v>2124.583146979235</v>
       </c>
     </row>
     <row r="38" spans="1:26">
@@ -1628,10 +1628,10 @@
         <v>37.098781754166666</v>
       </c>
       <c r="B38">
-        <v>-20758.217942523377</v>
+        <v>-22303.732977775417</v>
       </c>
       <c r="C38">
-        <v>176.66288789174283</v>
+        <v>2338.8626363762783</v>
       </c>
     </row>
     <row r="39" spans="1:26">
@@ -1639,10 +1639,10 @@
         <v>39.05129658333333</v>
       </c>
       <c r="B39">
-        <v>-20815.770097776793</v>
+        <v>-22494.433376419212</v>
       </c>
       <c r="C39">
-        <v>197.75783153799966</v>
+        <v>2546.865510271392</v>
       </c>
     </row>
     <row r="40" spans="1:26">
@@ -1650,10 +1650,10 @@
         <v>41.0038114125</v>
       </c>
       <c r="B40">
-        <v>-20838.674216468622</v>
+        <v>-22647.113308454293</v>
       </c>
       <c r="C40">
-        <v>218.68668543002858</v>
+        <v>2743.382954097288</v>
       </c>
     </row>
     <row r="41" spans="1:26">
@@ -1661,10 +1661,10 @@
         <v>42.956326241666666</v>
       </c>
       <c r="B41">
-        <v>-20820.241632622</v>
+        <v>-22751.789332519074</v>
       </c>
       <c r="C41">
-        <v>238.73250523449457</v>
+        <v>2923.3360620471194</v>
       </c>
     </row>
     <row r="42" spans="1:26">
@@ -1672,10 +1672,10 @@
         <v>44.90884107083333</v>
       </c>
       <c r="B42">
-        <v>-20755.591491882704</v>
+        <v>-22799.249974716393</v>
       </c>
       <c r="C42">
-        <v>257.1263545832731</v>
+        <v>3082.5454355538914</v>
       </c>
     </row>
     <row r="43" spans="1:26">
@@ -1683,10 +1683,10 @@
         <v>46.8613559</v>
       </c>
       <c r="B43">
-        <v>-20642.621001125444</v>
+        <v>-22782.143891614673</v>
       </c>
       <c r="C43">
-        <v>273.14011716776565</v>
+        <v>3218.549326920287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new version and params
</commit_message>
<xml_diff>
--- a/test/writer_output/Isosteric Heat Analysis.xlsx
+++ b/test/writer_output/Isosteric Heat Analysis.xlsx
@@ -14,6 +14,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Isosteric Heat Analysis" r:id="rId4" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,6 +23,44 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+  <si>
+    <t>Fitted, interpolated data</t>
+  </si>
+  <si>
+    <t>Sampled CC/CC</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>P[MPa]</t>
+  </si>
+  <si>
+    <t>Manipulated data for getting ∂ln(P)/∂(1/T)</t>
+  </si>
+  <si>
+    <t>1/T (K^-1)</t>
+  </si>
+  <si>
+    <t>ln(P[MPa])</t>
+  </si>
+  <si>
+    <t>Isosteric heats as a function of concentration</t>
+  </si>
+  <si>
+    <t>Conc (CC/CC)</t>
+  </si>
+  <si>
+    <t>ΔH_s (J/mol)</t>
+  </si>
+  <si>
+    <t>ΔH_s err (J/mol)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,4 +418,1278 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:Z43"/>
+  <sheetViews>
+    <sheetView tabSelected="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:26">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.001</v>
+      </c>
+      <c r="C2">
+        <v>1.9535148291666666</v>
+      </c>
+      <c r="D2">
+        <v>3.906029658333333</v>
+      </c>
+      <c r="E2">
+        <v>5.8585444875</v>
+      </c>
+      <c r="F2">
+        <v>7.811059316666666</v>
+      </c>
+      <c r="G2">
+        <v>9.763574145833333</v>
+      </c>
+      <c r="H2">
+        <v>11.716088975</v>
+      </c>
+      <c r="I2">
+        <v>13.668603804166668</v>
+      </c>
+      <c r="J2">
+        <v>15.621118633333333</v>
+      </c>
+      <c r="K2">
+        <v>17.5736334625</v>
+      </c>
+      <c r="L2">
+        <v>19.52614829166667</v>
+      </c>
+      <c r="M2">
+        <v>21.478663120833332</v>
+      </c>
+      <c r="N2">
+        <v>23.43117795</v>
+      </c>
+      <c r="O2">
+        <v>25.383692779166665</v>
+      </c>
+      <c r="P2">
+        <v>27.336207608333336</v>
+      </c>
+      <c r="Q2">
+        <v>29.2887224375</v>
+      </c>
+      <c r="R2">
+        <v>31.241237266666666</v>
+      </c>
+      <c r="S2">
+        <v>33.19375209583334</v>
+      </c>
+      <c r="T2">
+        <v>35.146266925</v>
+      </c>
+      <c r="U2">
+        <v>37.098781754166666</v>
+      </c>
+      <c r="V2">
+        <v>39.05129658333333</v>
+      </c>
+      <c r="W2">
+        <v>41.0038114125</v>
+      </c>
+      <c r="X2">
+        <v>42.956326241666666</v>
+      </c>
+      <c r="Y2">
+        <v>44.90884107083333</v>
+      </c>
+      <c r="Z2">
+        <v>46.8613559</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R3" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" t="s">
+        <v>3</v>
+      </c>
+      <c r="T3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" t="s">
+        <v>3</v>
+      </c>
+      <c r="V3" t="s">
+        <v>3</v>
+      </c>
+      <c r="W3" t="s">
+        <v>3</v>
+      </c>
+      <c r="X3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4">
+        <v>293.15</v>
+      </c>
+      <c r="B4">
+        <v>9.119028296170422e-6</v>
+      </c>
+      <c r="C4">
+        <v>0.018391395045482872</v>
+      </c>
+      <c r="D4">
+        <v>0.03800063980479852</v>
+      </c>
+      <c r="E4">
+        <v>0.05895650858192524</v>
+      </c>
+      <c r="F4">
+        <v>0.08139361794483305</v>
+      </c>
+      <c r="G4">
+        <v>0.10546374226553795</v>
+      </c>
+      <c r="H4">
+        <v>0.13133835636167818</v>
+      </c>
+      <c r="I4">
+        <v>0.15921157391688495</v>
+      </c>
+      <c r="J4">
+        <v>0.18930353366924638</v>
+      </c>
+      <c r="K4">
+        <v>0.2218642845351649</v>
+      </c>
+      <c r="L4">
+        <v>0.2571782145127691</v>
+      </c>
+      <c r="M4">
+        <v>0.29556905287542284</v>
+      </c>
+      <c r="N4">
+        <v>0.33740544571569475</v>
+      </c>
+      <c r="O4">
+        <v>0.3831070541686949</v>
+      </c>
+      <c r="P4">
+        <v>0.43315104303962343</v>
+      </c>
+      <c r="Q4">
+        <v>0.488078703082626</v>
+      </c>
+      <c r="R4">
+        <v>0.5485017693817901</v>
+      </c>
+      <c r="S4">
+        <v>0.615107749153492</v>
+      </c>
+      <c r="T4">
+        <v>0.68866325041921</v>
+      </c>
+      <c r="U4">
+        <v>0.7700139227090961</v>
+      </c>
+      <c r="V4">
+        <v>0.8600792321815738</v>
+      </c>
+      <c r="W4">
+        <v>0.9598400023437031</v>
+      </c>
+      <c r="X4">
+        <v>1.070316635349533</v>
+      </c>
+      <c r="Y4">
+        <v>1.1925364269474923</v>
+      </c>
+      <c r="Z4">
+        <v>1.3274896392376172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5">
+        <v>300.15</v>
+      </c>
+      <c r="B5">
+        <v>1.0965195990091104e-5</v>
+      </c>
+      <c r="C5">
+        <v>0.022131436836201182</v>
+      </c>
+      <c r="D5">
+        <v>0.045766170670456886</v>
+      </c>
+      <c r="E5">
+        <v>0.07106892993093257</v>
+      </c>
+      <c r="F5">
+        <v>0.09821389842341031</v>
+      </c>
+      <c r="G5">
+        <v>0.12739896036981394</v>
+      </c>
+      <c r="H5">
+        <v>0.1588495766923801</v>
+      </c>
+      <c r="I5">
+        <v>0.1928233708826446</v>
+      </c>
+      <c r="J5">
+        <v>0.22961555629574612</v>
+      </c>
+      <c r="K5">
+        <v>0.269565355834171</v>
+      </c>
+      <c r="L5">
+        <v>0.31306358231659664</v>
+      </c>
+      <c r="M5">
+        <v>0.3605615593032984</v>
+      </c>
+      <c r="N5">
+        <v>0.41258156074680385</v>
+      </c>
+      <c r="O5">
+        <v>0.46972892193805754</v>
+      </c>
+      <c r="P5">
+        <v>0.532705905343227</v>
+      </c>
+      <c r="Q5">
+        <v>0.6023272648613003</v>
+      </c>
+      <c r="R5">
+        <v>0.679537199821544</v>
+      </c>
+      <c r="S5">
+        <v>0.7654269702565001</v>
+      </c>
+      <c r="T5">
+        <v>0.8612517906350058</v>
+      </c>
+      <c r="U5">
+        <v>0.9684446658464305</v>
+      </c>
+      <c r="V5">
+        <v>1.088623554900231</v>
+      </c>
+      <c r="W5">
+        <v>1.2235867286315227</v>
+      </c>
+      <c r="X5">
+        <v>1.3752897350451516</v>
+      </c>
+      <c r="Y5">
+        <v>1.5457966608784894</v>
+      </c>
+      <c r="Z5">
+        <v>1.7371994464902663</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6">
+        <v>308.15</v>
+      </c>
+      <c r="B6">
+        <v>1.2890321023727155e-5</v>
+      </c>
+      <c r="C6">
+        <v>0.026157627651847887</v>
+      </c>
+      <c r="D6">
+        <v>0.054401479686169055</v>
+      </c>
+      <c r="E6">
+        <v>0.08499016592290676</v>
+      </c>
+      <c r="F6">
+        <v>0.1182060402362688</v>
+      </c>
+      <c r="G6">
+        <v>0.15437439687535437</v>
+      </c>
+      <c r="H6">
+        <v>0.19387088891352675</v>
+      </c>
+      <c r="I6">
+        <v>0.23713020560857104</v>
+      </c>
+      <c r="J6">
+        <v>0.2846561325326306</v>
+      </c>
+      <c r="K6">
+        <v>0.33703305949405277</v>
+      </c>
+      <c r="L6">
+        <v>0.39493888258541165</v>
+      </c>
+      <c r="M6">
+        <v>0.459159033973199</v>
+      </c>
+      <c r="N6">
+        <v>0.5306010202317961</v>
+      </c>
+      <c r="O6">
+        <v>0.6103083018201666</v>
+      </c>
+      <c r="P6">
+        <v>0.6994715503091371</v>
+      </c>
+      <c r="Q6">
+        <v>0.7994342572943302</v>
+      </c>
+      <c r="R6">
+        <v>0.9116884141735291</v>
+      </c>
+      <c r="S6">
+        <v>1.037854797426806</v>
+      </c>
+      <c r="T6">
+        <v>1.1796418361825063</v>
+      </c>
+      <c r="U6">
+        <v>1.3387779949868457</v>
+      </c>
+      <c r="V6">
+        <v>1.5169160975954334</v>
+      </c>
+      <c r="W6">
+        <v>1.7155146036246816</v>
+      </c>
+      <c r="X6">
+        <v>1.935709665603194</v>
+      </c>
+      <c r="Y6">
+        <v>2.1781998613292473</v>
+      </c>
+      <c r="Z6">
+        <v>2.443168373187182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7">
+        <v>323.15</v>
+      </c>
+      <c r="B7">
+        <v>1.8473750063392738e-5</v>
+      </c>
+      <c r="C7">
+        <v>0.03742548090100247</v>
+      </c>
+      <c r="D7">
+        <v>0.07769610638778919</v>
+      </c>
+      <c r="E7">
+        <v>0.12114688103380995</v>
+      </c>
+      <c r="F7">
+        <v>0.16813832487272748</v>
+      </c>
+      <c r="G7">
+        <v>0.21908185899382918</v>
+      </c>
+      <c r="H7">
+        <v>0.27444777774580387</v>
+      </c>
+      <c r="I7">
+        <v>0.33477437348934974</v>
+      </c>
+      <c r="J7">
+        <v>0.4006782641287994</v>
+      </c>
+      <c r="K7">
+        <v>0.4728658937146207</v>
+      </c>
+      <c r="L7">
+        <v>0.5521460388223153</v>
+      </c>
+      <c r="M7">
+        <v>0.639442932047627</v>
+      </c>
+      <c r="N7">
+        <v>0.7358092770039117</v>
+      </c>
+      <c r="O7">
+        <v>0.8424379435924141</v>
+      </c>
+      <c r="P7">
+        <v>0.9606704751589408</v>
+      </c>
+      <c r="Q7">
+        <v>1.0919997208629306</v>
+      </c>
+      <c r="R7">
+        <v>1.2380630097120604</v>
+      </c>
+      <c r="S7">
+        <v>1.400621515003608</v>
+      </c>
+      <c r="T7">
+        <v>1.5815212024126364</v>
+      </c>
+      <c r="U7">
+        <v>1.7826315713529446</v>
+      </c>
+      <c r="V7">
+        <v>2.005760899003269</v>
+      </c>
+      <c r="W7">
+        <v>2.2525512184209866</v>
+      </c>
+      <c r="X7">
+        <v>2.524362379079606</v>
+      </c>
+      <c r="Y7">
+        <v>2.8221606553925147</v>
+      </c>
+      <c r="Z7">
+        <v>3.1464308987103604</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0.001</v>
+      </c>
+      <c r="C10">
+        <v>1.9535148291666666</v>
+      </c>
+      <c r="D10">
+        <v>3.906029658333333</v>
+      </c>
+      <c r="E10">
+        <v>5.8585444875</v>
+      </c>
+      <c r="F10">
+        <v>7.811059316666666</v>
+      </c>
+      <c r="G10">
+        <v>9.763574145833333</v>
+      </c>
+      <c r="H10">
+        <v>11.716088975</v>
+      </c>
+      <c r="I10">
+        <v>13.668603804166668</v>
+      </c>
+      <c r="J10">
+        <v>15.621118633333333</v>
+      </c>
+      <c r="K10">
+        <v>17.5736334625</v>
+      </c>
+      <c r="L10">
+        <v>19.52614829166667</v>
+      </c>
+      <c r="M10">
+        <v>21.478663120833332</v>
+      </c>
+      <c r="N10">
+        <v>23.43117795</v>
+      </c>
+      <c r="O10">
+        <v>25.383692779166665</v>
+      </c>
+      <c r="P10">
+        <v>27.336207608333336</v>
+      </c>
+      <c r="Q10">
+        <v>29.2887224375</v>
+      </c>
+      <c r="R10">
+        <v>31.241237266666666</v>
+      </c>
+      <c r="S10">
+        <v>33.19375209583334</v>
+      </c>
+      <c r="T10">
+        <v>35.146266925</v>
+      </c>
+      <c r="U10">
+        <v>37.098781754166666</v>
+      </c>
+      <c r="V10">
+        <v>39.05129658333333</v>
+      </c>
+      <c r="W10">
+        <v>41.0038114125</v>
+      </c>
+      <c r="X10">
+        <v>42.956326241666666</v>
+      </c>
+      <c r="Y10">
+        <v>44.90884107083333</v>
+      </c>
+      <c r="Z10">
+        <v>46.8613559</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" t="s">
+        <v>6</v>
+      </c>
+      <c r="N11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" t="s">
+        <v>6</v>
+      </c>
+      <c r="S11" t="s">
+        <v>6</v>
+      </c>
+      <c r="T11" t="s">
+        <v>6</v>
+      </c>
+      <c r="U11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V11" t="s">
+        <v>6</v>
+      </c>
+      <c r="W11" t="s">
+        <v>6</v>
+      </c>
+      <c r="X11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12">
+        <v>0.003411222923418046</v>
+      </c>
+      <c r="B12">
+        <v>-11.605147306027055</v>
+      </c>
+      <c r="C12">
+        <v>-3.995872384326091</v>
+      </c>
+      <c r="D12">
+        <v>-3.2701522824291094</v>
+      </c>
+      <c r="E12">
+        <v>-2.8309552495789054</v>
+      </c>
+      <c r="F12">
+        <v>-2.5084584126734972</v>
+      </c>
+      <c r="G12">
+        <v>-2.2493880603440455</v>
+      </c>
+      <c r="H12">
+        <v>-2.029978412674971</v>
+      </c>
+      <c r="I12">
+        <v>-1.8375213077314607</v>
+      </c>
+      <c r="J12">
+        <v>-1.6644035539086177</v>
+      </c>
+      <c r="K12">
+        <v>-1.5056894149714783</v>
+      </c>
+      <c r="L12">
+        <v>-1.3579859927225832</v>
+      </c>
+      <c r="M12">
+        <v>-1.2188527879617348</v>
+      </c>
+      <c r="N12">
+        <v>-1.0864699687643187</v>
+      </c>
+      <c r="O12">
+        <v>-0.9594408140577052</v>
+      </c>
+      <c r="P12">
+        <v>-0.8366687826155881</v>
+      </c>
+      <c r="Q12">
+        <v>-0.7172786093240364</v>
+      </c>
+      <c r="R12">
+        <v>-0.6005647734164671</v>
+      </c>
+      <c r="S12">
+        <v>-0.4859578246460787</v>
+      </c>
+      <c r="T12">
+        <v>-0.37300287865207166</v>
+      </c>
+      <c r="U12">
+        <v>-0.2613466828574903</v>
+      </c>
+      <c r="V12">
+        <v>-0.15073076353464188</v>
+      </c>
+      <c r="W12">
+        <v>-0.04098867263558969</v>
+      </c>
+      <c r="X12">
+        <v>0.06795452558527898</v>
+      </c>
+      <c r="Y12">
+        <v>0.17608249002031057</v>
+      </c>
+      <c r="Z12">
+        <v>0.28328966938607403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13">
+        <v>0.003331667499583542</v>
+      </c>
+      <c r="B13">
+        <v>-11.420784302100849</v>
+      </c>
+      <c r="C13">
+        <v>-3.81075619995043</v>
+      </c>
+      <c r="D13">
+        <v>-3.084210092434169</v>
+      </c>
+      <c r="E13">
+        <v>-2.6441050288075134</v>
+      </c>
+      <c r="F13">
+        <v>-2.3206075418297756</v>
+      </c>
+      <c r="G13">
+        <v>-2.060431696239898</v>
+      </c>
+      <c r="H13">
+        <v>-1.8397975830962243</v>
+      </c>
+      <c r="I13">
+        <v>-1.6459806858810546</v>
+      </c>
+      <c r="J13">
+        <v>-1.4713488629305844</v>
+      </c>
+      <c r="K13">
+        <v>-1.3109444102998593</v>
+      </c>
+      <c r="L13">
+        <v>-1.1613489706801106</v>
+      </c>
+      <c r="M13">
+        <v>-1.0200925759383102</v>
+      </c>
+      <c r="N13">
+        <v>-0.8853213697294672</v>
+      </c>
+      <c r="O13">
+        <v>-0.7555995125030412</v>
+      </c>
+      <c r="P13">
+        <v>-0.6297857794378303</v>
+      </c>
+      <c r="Q13">
+        <v>-0.5069543520485047</v>
+      </c>
+      <c r="R13">
+        <v>-0.38634330101520237</v>
+      </c>
+      <c r="S13">
+        <v>-0.2673214697985593</v>
+      </c>
+      <c r="T13">
+        <v>-0.1493683775446672</v>
+      </c>
+      <c r="U13">
+        <v>-0.03206393163777815</v>
+      </c>
+      <c r="V13">
+        <v>0.08491410457574017</v>
+      </c>
+      <c r="W13">
+        <v>0.20178648706998767</v>
+      </c>
+      <c r="X13">
+        <v>0.31866442531742684</v>
+      </c>
+      <c r="Y13">
+        <v>0.43553941556311576</v>
+      </c>
+      <c r="Z13">
+        <v>0.5522743030567119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14">
+        <v>0.0032451728054518907</v>
+      </c>
+      <c r="B14">
+        <v>-11.259033836456956</v>
+      </c>
+      <c r="C14">
+        <v>-3.643614442596813</v>
+      </c>
+      <c r="D14">
+        <v>-2.911363925376755</v>
+      </c>
+      <c r="E14">
+        <v>-2.4652197242096325</v>
+      </c>
+      <c r="F14">
+        <v>-2.135326073486108</v>
+      </c>
+      <c r="G14">
+        <v>-1.868374478487823</v>
+      </c>
+      <c r="H14">
+        <v>-1.6405628625405537</v>
+      </c>
+      <c r="I14">
+        <v>-1.43914589795339</v>
+      </c>
+      <c r="J14">
+        <v>-1.2564733797010779</v>
+      </c>
+      <c r="K14">
+        <v>-1.087574254052325</v>
+      </c>
+      <c r="L14">
+        <v>-0.9290242536844393</v>
+      </c>
+      <c r="M14">
+        <v>-0.7783586496872219</v>
+      </c>
+      <c r="N14">
+        <v>-0.6337449144914354</v>
+      </c>
+      <c r="O14">
+        <v>-0.4937910366728759</v>
+      </c>
+      <c r="P14">
+        <v>-0.35743015717027365</v>
+      </c>
+      <c r="Q14">
+        <v>-0.22385097986487862</v>
+      </c>
+      <c r="R14">
+        <v>-0.09245699840936435</v>
+      </c>
+      <c r="S14">
+        <v>0.03715588808655996</v>
+      </c>
+      <c r="T14">
+        <v>0.1652108637445336</v>
+      </c>
+      <c r="U14">
+        <v>0.2917572538492102</v>
+      </c>
+      <c r="V14">
+        <v>0.41667939072572685</v>
+      </c>
+      <c r="W14">
+        <v>0.5397130960313329</v>
+      </c>
+      <c r="X14">
+        <v>0.6604740114942905</v>
+      </c>
+      <c r="Y14">
+        <v>0.7784987839964441</v>
+      </c>
+      <c r="Z14">
+        <v>0.8932957105667424</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15">
+        <v>0.0030945381401825778</v>
+      </c>
+      <c r="B15">
+        <v>-10.899159748986126</v>
+      </c>
+      <c r="C15">
+        <v>-3.285403499032817</v>
+      </c>
+      <c r="D15">
+        <v>-2.5549501337033895</v>
+      </c>
+      <c r="E15">
+        <v>-2.110751576716211</v>
+      </c>
+      <c r="F15">
+        <v>-1.7829682760180394</v>
+      </c>
+      <c r="G15">
+        <v>-1.5183098336460303</v>
+      </c>
+      <c r="H15">
+        <v>-1.2929942811376074</v>
+      </c>
+      <c r="I15">
+        <v>-1.0942984860402398</v>
+      </c>
+      <c r="J15">
+        <v>-0.9145965075610273</v>
+      </c>
+      <c r="K15">
+        <v>-0.7489434534924628</v>
+      </c>
+      <c r="L15">
+        <v>-0.5939427046117786</v>
+      </c>
+      <c r="M15">
+        <v>-0.44715790033829933</v>
+      </c>
+      <c r="N15">
+        <v>-0.306784328339963</v>
+      </c>
+      <c r="O15">
+        <v>-0.17145527692553925</v>
+      </c>
+      <c r="P15">
+        <v>-0.04012382667225934</v>
+      </c>
+      <c r="Q15">
+        <v>0.08801062170265372</v>
+      </c>
+      <c r="R15">
+        <v>0.21354806934207468</v>
+      </c>
+      <c r="S15">
+        <v>0.33691607739761303</v>
+      </c>
+      <c r="T15">
+        <v>0.4583871701944943</v>
+      </c>
+      <c r="U15">
+        <v>0.5780906834030081</v>
+      </c>
+      <c r="V15">
+        <v>0.6960234895160966</v>
+      </c>
+      <c r="W15">
+        <v>0.8120634487195262</v>
+      </c>
+      <c r="X15">
+        <v>0.9259885077011974</v>
+      </c>
+      <c r="Y15">
+        <v>1.0375027814319202</v>
+      </c>
+      <c r="Z15">
+        <v>1.1462687624248866</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
+      <c r="A19">
+        <v>0.001</v>
+      </c>
+      <c r="B19">
+        <v>-18378.57581055563</v>
+      </c>
+      <c r="C19">
+        <v>579.513410356215</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
+      <c r="A20">
+        <v>1.9535148291666666</v>
+      </c>
+      <c r="B20">
+        <v>-18514.235349113515</v>
+      </c>
+      <c r="C20">
+        <v>496.3133063113973</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
+      <c r="A21">
+        <v>3.906029658333333</v>
+      </c>
+      <c r="B21">
+        <v>-18657.396694606457</v>
+      </c>
+      <c r="C21">
+        <v>408.4859770731027</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
+      <c r="A22">
+        <v>5.8585444875</v>
+      </c>
+      <c r="B22">
+        <v>-18808.527027553635</v>
+      </c>
+      <c r="C22">
+        <v>316.3657642400436</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
+      <c r="A23">
+        <v>7.811059316666666</v>
+      </c>
+      <c r="B23">
+        <v>-18968.09808718258</v>
+      </c>
+      <c r="C23">
+        <v>221.76317513179177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
+      <c r="A24">
+        <v>9.763574145833333</v>
+      </c>
+      <c r="B24">
+        <v>-19136.574086069995</v>
+      </c>
+      <c r="C24">
+        <v>133.8686920886433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25">
+        <v>11.716088975</v>
+      </c>
+      <c r="B25">
+        <v>-19314.394300186224</v>
+      </c>
+      <c r="C25">
+        <v>103.96776402404235</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="A26">
+        <v>13.668603804166668</v>
+      </c>
+      <c r="B26">
+        <v>-19501.94852927425</v>
+      </c>
+      <c r="C26">
+        <v>182.08245031137267</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27">
+        <v>15.621118633333333</v>
+      </c>
+      <c r="B27">
+        <v>-19699.543131531842</v>
+      </c>
+      <c r="C27">
+        <v>301.9546067034061</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="A28">
+        <v>17.5736334625</v>
+      </c>
+      <c r="B28">
+        <v>-19907.354784993036</v>
+      </c>
+      <c r="C28">
+        <v>438.2813891644411</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="A29">
+        <v>19.52614829166667</v>
+      </c>
+      <c r="B29">
+        <v>-20125.368576459005</v>
+      </c>
+      <c r="C29">
+        <v>586.6344216766888</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="A30">
+        <v>21.478663120833332</v>
+      </c>
+      <c r="B30">
+        <v>-20353.296595538857</v>
+      </c>
+      <c r="C30">
+        <v>746.0290239284012</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="A31">
+        <v>23.43117795</v>
+      </c>
+      <c r="B31">
+        <v>-20590.473158167642</v>
+      </c>
+      <c r="C31">
+        <v>916.189265828536</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26">
+      <c r="A32">
+        <v>25.383692779166665</v>
+      </c>
+      <c r="B32">
+        <v>-20835.72351460252</v>
+      </c>
+      <c r="C32">
+        <v>1096.890090251264</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26">
+      <c r="A33">
+        <v>27.336207608333336</v>
+      </c>
+      <c r="B33">
+        <v>-21087.20505574941</v>
+      </c>
+      <c r="C33">
+        <v>1287.6808536382866</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26">
+      <c r="A34">
+        <v>29.2887224375</v>
+      </c>
+      <c r="B34">
+        <v>-21342.22451509101</v>
+      </c>
+      <c r="C34">
+        <v>1487.6929960566301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26">
+      <c r="A35">
+        <v>31.241237266666666</v>
+      </c>
+      <c r="B35">
+        <v>-21597.042519102582</v>
+      </c>
+      <c r="C35">
+        <v>1695.466411969708</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26">
+      <c r="A36">
+        <v>33.19375209583334</v>
+      </c>
+      <c r="B36">
+        <v>-21846.688900603258</v>
+      </c>
+      <c r="C36">
+        <v>1908.7901861427886</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26">
+      <c r="A37">
+        <v>35.146266925</v>
+      </c>
+      <c r="B37">
+        <v>-22084.82827389003</v>
+      </c>
+      <c r="C37">
+        <v>2124.5831469199175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26">
+      <c r="A38">
+        <v>37.098781754166666</v>
+      </c>
+      <c r="B38">
+        <v>-22303.732977683034</v>
+      </c>
+      <c r="C38">
+        <v>2338.8626363207395</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26">
+      <c r="A39">
+        <v>39.05129658333333</v>
+      </c>
+      <c r="B39">
+        <v>-22494.43337632375</v>
+      </c>
+      <c r="C39">
+        <v>2546.8655102217203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26">
+      <c r="A40">
+        <v>41.0038114125</v>
+      </c>
+      <c r="B40">
+        <v>-22647.113308360218</v>
+      </c>
+      <c r="C40">
+        <v>2743.3829540558895</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26">
+      <c r="A41">
+        <v>42.956326241666666</v>
+      </c>
+      <c r="B41">
+        <v>-22751.789332432345</v>
+      </c>
+      <c r="C41">
+        <v>2923.336062016438</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26">
+      <c r="A42">
+        <v>44.90884107083333</v>
+      </c>
+      <c r="B42">
+        <v>-22799.249974643626</v>
+      </c>
+      <c r="C42">
+        <v>3082.5454355357806</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26">
+      <c r="A43">
+        <v>46.8613559</v>
+      </c>
+      <c r="B43">
+        <v>-22782.143891563755</v>
+      </c>
+      <c r="C43">
+        <v>3218.5493269153303</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
more info in isosteric heats
</commit_message>
<xml_diff>
--- a/test/writer_output/Isosteric Heat Analysis.xlsx
+++ b/test/writer_output/Isosteric Heat Analysis.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Membrane Libraries\SorptionModels.jl\test\writer_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E5E84F-DB8F-485A-9BB1-8FA1F7071C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Isosteric Heat Analysis" r:id="rId4" sheetId="2"/>
+    <sheet name="Isosteric Heat Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="15">
   <si>
     <t>Fitted, interpolated data</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>ΔH_s err (J/mol)</t>
+  </si>
+  <si>
+    <t>ΔS_s (J/molK)</t>
+  </si>
+  <si>
+    <t>ΔS_s err (J/molK)</t>
+  </si>
+  <si>
+    <t>S0 (J/molK) (S0 = exp(ΔS_s/R))</t>
+  </si>
+  <si>
+    <t>S0 err (J/molK)</t>
   </si>
 </sst>
 </file>
@@ -111,6 +123,1269 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Isosteric Heat Analysis'!$D$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ΔS_s (J/molK)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Isosteric Heat Analysis'!$E$19:$E$43</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="25"/>
+                  <c:pt idx="0">
+                    <c:v>1.8966067800595494</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.6243130270365327</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.3368754886964236</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.0353883839677958</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.7257770640095399</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.43811974756021632</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.34026126510933347</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.59591167972822701</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.98822416204635255</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.4343886429690142</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.9199121222827598</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.4415719802482032</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.9984651646285174</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.5898551180582992</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.2142669935145367</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>4.8688582050823435</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>5.5488501816177136</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>6.2470071340096585</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>6.9532451350378901</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>7.6545299114772982</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>8.3352728483318241</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>8.9784267593806728</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>9.5673696182542489</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>10.088423267522195</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>10.533531004280835</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Isosteric Heat Analysis'!$E$19:$E$43</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="25"/>
+                  <c:pt idx="0">
+                    <c:v>1.8966067800595494</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.6243130270365327</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.3368754886964236</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.0353883839677958</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.7257770640095399</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.43811974756021632</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.34026126510933347</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.59591167972822701</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.98822416204635255</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>1.4343886429690142</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.9199121222827598</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.4415719802482032</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.9984651646285174</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.5898551180582992</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.2142669935145367</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>4.8688582050823435</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>5.5488501816177136</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>6.2470071340096585</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>6.9532451350378901</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>7.6545299114772982</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>8.3352728483318241</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>8.9784267593806728</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>9.5673696182542489</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>10.088423267522195</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>10.533531004280835</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Isosteric Heat Analysis'!$A$19:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9535148291666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9060296583333329</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8585444874999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8110593166666664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.7635741458333332</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.716088975</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.668603804166668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.621118633333333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.573633462499998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.526148291666669</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.478663120833332</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>23.431177949999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25.383692779166665</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.336207608333336</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29.288722437499999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.241237266666666</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>33.193752095833339</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>35.146266924999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37.098781754166666</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>39.051296583333333</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41.003811412499999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>42.956326241666666</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>44.908841070833333</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>46.8613559</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Isosteric Heat Analysis'!$D$19:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>-23.623738341661344</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-24.356229144180258</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-25.122544341889313</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-25.924735401642966</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-26.764901034589581</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-27.645147515681504</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-28.567530498312387</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-29.533971951452347</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-30.54614408494443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-31.605310131500403</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-32.71210982080224</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-33.866275743502754</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-35.06626638401891</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-36.308803820153599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-37.588311169961109</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-38.89625992847386</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-40.220464057396264</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-41.544399070941012</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-42.846679969364715</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-44.100893352603094</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-45.276025148907131</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-46.337720616959189</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-47.250516866640211</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-47.980978048356143</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-48.501368268275641</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E1F9-457C-A2B0-C725BE4A981D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="619430191"/>
+        <c:axId val="1774364991"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="619430191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1774364991"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1774364991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="619430191"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>747712</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EEA0F38-8D7B-41A7-11FC-24E7BB6E7BED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,51 +1684,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DBF207-2C3C-4A8C-8C04-F327B465D251}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E7E0FF-828D-4860-A1B0-20AC06D00F28}">
   <dimension ref="A1:Z43"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="C2">
         <v>1.9535148291666666</v>
       </c>
       <c r="D2">
-        <v>3.906029658333333</v>
+        <v>3.9060296583333329</v>
       </c>
       <c r="E2">
-        <v>5.8585444875</v>
+        <v>5.8585444874999997</v>
       </c>
       <c r="F2">
-        <v>7.811059316666666</v>
+        <v>7.8110593166666664</v>
       </c>
       <c r="G2">
-        <v>9.763574145833333</v>
+        <v>9.7635741458333332</v>
       </c>
       <c r="H2">
         <v>11.716088975</v>
@@ -465,16 +1742,16 @@
         <v>15.621118633333333</v>
       </c>
       <c r="K2">
-        <v>17.5736334625</v>
+        <v>17.573633462499998</v>
       </c>
       <c r="L2">
-        <v>19.52614829166667</v>
+        <v>19.526148291666669</v>
       </c>
       <c r="M2">
         <v>21.478663120833332</v>
       </c>
       <c r="N2">
-        <v>23.43117795</v>
+        <v>23.431177949999999</v>
       </c>
       <c r="O2">
         <v>25.383692779166665</v>
@@ -483,37 +1760,37 @@
         <v>27.336207608333336</v>
       </c>
       <c r="Q2">
-        <v>29.2887224375</v>
+        <v>29.288722437499999</v>
       </c>
       <c r="R2">
         <v>31.241237266666666</v>
       </c>
       <c r="S2">
-        <v>33.19375209583334</v>
+        <v>33.193752095833339</v>
       </c>
       <c r="T2">
-        <v>35.146266925</v>
+        <v>35.146266924999999</v>
       </c>
       <c r="U2">
         <v>37.098781754166666</v>
       </c>
       <c r="V2">
-        <v>39.05129658333333</v>
+        <v>39.051296583333333</v>
       </c>
       <c r="W2">
-        <v>41.0038114125</v>
+        <v>41.003811412499999</v>
       </c>
       <c r="X2">
         <v>42.956326241666666</v>
       </c>
       <c r="Y2">
-        <v>44.90884107083333</v>
+        <v>44.908841070833333</v>
       </c>
       <c r="Z2">
         <v>46.8613559</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -593,24 +1870,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>293.15</v>
+        <v>293.14999999999998</v>
       </c>
       <c r="B4">
-        <v>9.119028296170422e-6</v>
+        <v>9.1190282961704218E-6</v>
       </c>
       <c r="C4">
-        <v>0.018391395045482872</v>
+        <v>1.8391395045482872E-2</v>
       </c>
       <c r="D4">
-        <v>0.03800063980479852</v>
+        <v>3.8000639804798522E-2</v>
       </c>
       <c r="E4">
-        <v>0.05895650858192524</v>
+        <v>5.8956508581925242E-2</v>
       </c>
       <c r="F4">
-        <v>0.08139361794483305</v>
+        <v>8.1393617944833047E-2</v>
       </c>
       <c r="G4">
         <v>0.10546374226553795</v>
@@ -625,10 +1902,10 @@
         <v>0.18930353366924638</v>
       </c>
       <c r="K4">
-        <v>0.2218642845351649</v>
+        <v>0.22186428453516491</v>
       </c>
       <c r="L4">
-        <v>0.2571782145127691</v>
+        <v>0.25717821451276912</v>
       </c>
       <c r="M4">
         <v>0.29556905287542284</v>
@@ -637,31 +1914,31 @@
         <v>0.33740544571569475</v>
       </c>
       <c r="O4">
-        <v>0.3831070541686949</v>
+        <v>0.38310705416869489</v>
       </c>
       <c r="P4">
         <v>0.43315104303962343</v>
       </c>
       <c r="Q4">
-        <v>0.488078703082626</v>
+        <v>0.48807870308262602</v>
       </c>
       <c r="R4">
-        <v>0.5485017693817901</v>
+        <v>0.54850176938179007</v>
       </c>
       <c r="S4">
-        <v>0.615107749153492</v>
+        <v>0.61510774915349198</v>
       </c>
       <c r="T4">
-        <v>0.68866325041921</v>
+        <v>0.68866325041920995</v>
       </c>
       <c r="U4">
-        <v>0.7700139227090961</v>
+        <v>0.77001392270909608</v>
       </c>
       <c r="V4">
-        <v>0.8600792321815738</v>
+        <v>0.86007923218157378</v>
       </c>
       <c r="W4">
-        <v>0.9598400023437031</v>
+        <v>0.95984000234370315</v>
       </c>
       <c r="X4">
         <v>1.070316635349533</v>
@@ -673,45 +1950,45 @@
         <v>1.3274896392376172</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>300.15</v>
+        <v>300.14999999999998</v>
       </c>
       <c r="B5">
-        <v>1.0965195990091104e-5</v>
+        <v>1.0965195990091104E-5</v>
       </c>
       <c r="C5">
-        <v>0.022131436836201182</v>
+        <v>2.2131436836201182E-2</v>
       </c>
       <c r="D5">
-        <v>0.045766170670456886</v>
+        <v>4.5766170670456886E-2</v>
       </c>
       <c r="E5">
-        <v>0.07106892993093257</v>
+        <v>7.106892993093257E-2</v>
       </c>
       <c r="F5">
-        <v>0.09821389842341031</v>
+        <v>9.8213898423410315E-2</v>
       </c>
       <c r="G5">
         <v>0.12739896036981394</v>
       </c>
       <c r="H5">
-        <v>0.1588495766923801</v>
+        <v>0.15884957669238009</v>
       </c>
       <c r="I5">
-        <v>0.1928233708826446</v>
+        <v>0.19282337088264459</v>
       </c>
       <c r="J5">
         <v>0.22961555629574612</v>
       </c>
       <c r="K5">
-        <v>0.269565355834171</v>
+        <v>0.26956535583417102</v>
       </c>
       <c r="L5">
         <v>0.31306358231659664</v>
       </c>
       <c r="M5">
-        <v>0.3605615593032984</v>
+        <v>0.36056155930329842</v>
       </c>
       <c r="N5">
         <v>0.41258156074680385</v>
@@ -720,22 +1997,22 @@
         <v>0.46972892193805754</v>
       </c>
       <c r="P5">
-        <v>0.532705905343227</v>
+        <v>0.53270590534322704</v>
       </c>
       <c r="Q5">
-        <v>0.6023272648613003</v>
+        <v>0.60232726486130028</v>
       </c>
       <c r="R5">
-        <v>0.679537199821544</v>
+        <v>0.67953719982154404</v>
       </c>
       <c r="S5">
-        <v>0.7654269702565001</v>
+        <v>0.76542697025650008</v>
       </c>
       <c r="T5">
-        <v>0.8612517906350058</v>
+        <v>0.86125179063500579</v>
       </c>
       <c r="U5">
-        <v>0.9684446658464305</v>
+        <v>0.96844466584643052</v>
       </c>
       <c r="V5">
         <v>1.088623554900231</v>
@@ -753,24 +2030,24 @@
         <v>1.7371994464902663</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>308.15</v>
+        <v>308.14999999999998</v>
       </c>
       <c r="B6">
-        <v>1.2890321023727155e-5</v>
+        <v>1.2890321023727155E-5</v>
       </c>
       <c r="C6">
-        <v>0.026157627651847887</v>
+        <v>2.6157627651847887E-2</v>
       </c>
       <c r="D6">
-        <v>0.054401479686169055</v>
+        <v>5.4401479686169055E-2</v>
       </c>
       <c r="E6">
-        <v>0.08499016592290676</v>
+        <v>8.4990165922906757E-2</v>
       </c>
       <c r="F6">
-        <v>0.1182060402362688</v>
+        <v>0.11820604023626879</v>
       </c>
       <c r="G6">
         <v>0.15437439687535437</v>
@@ -782,7 +2059,7 @@
         <v>0.23713020560857104</v>
       </c>
       <c r="J6">
-        <v>0.2846561325326306</v>
+        <v>0.28465613253263061</v>
       </c>
       <c r="K6">
         <v>0.33703305949405277</v>
@@ -791,10 +2068,10 @@
         <v>0.39493888258541165</v>
       </c>
       <c r="M6">
-        <v>0.459159033973199</v>
+        <v>0.45915903397319902</v>
       </c>
       <c r="N6">
-        <v>0.5306010202317961</v>
+        <v>0.53060102023179612</v>
       </c>
       <c r="O6">
         <v>0.6103083018201666</v>
@@ -803,10 +2080,10 @@
         <v>0.6994715503091371</v>
       </c>
       <c r="Q6">
-        <v>0.7994342572943302</v>
+        <v>0.79943425729433015</v>
       </c>
       <c r="R6">
-        <v>0.9116884141735291</v>
+        <v>0.91168841417352908</v>
       </c>
       <c r="S6">
         <v>1.037854797426806</v>
@@ -830,21 +2107,21 @@
         <v>2.1781998613292473</v>
       </c>
       <c r="Z6">
-        <v>2.443168373187182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26">
+        <v>2.4431683731871821</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>323.15</v>
+        <v>323.14999999999998</v>
       </c>
       <c r="B7">
-        <v>1.8473750063392738e-5</v>
+        <v>1.8473750063392738E-5</v>
       </c>
       <c r="C7">
-        <v>0.03742548090100247</v>
+        <v>3.7425480901002471E-2</v>
       </c>
       <c r="D7">
-        <v>0.07769610638778919</v>
+        <v>7.7696106387789191E-2</v>
       </c>
       <c r="E7">
         <v>0.12114688103380995</v>
@@ -862,25 +2139,25 @@
         <v>0.33477437348934974</v>
       </c>
       <c r="J7">
-        <v>0.4006782641287994</v>
+        <v>0.40067826412879942</v>
       </c>
       <c r="K7">
-        <v>0.4728658937146207</v>
+        <v>0.47286589371462068</v>
       </c>
       <c r="L7">
-        <v>0.5521460388223153</v>
+        <v>0.55214603882231528</v>
       </c>
       <c r="M7">
-        <v>0.639442932047627</v>
+        <v>0.63944293204762703</v>
       </c>
       <c r="N7">
-        <v>0.7358092770039117</v>
+        <v>0.73580927700391174</v>
       </c>
       <c r="O7">
-        <v>0.8424379435924141</v>
+        <v>0.84243794359241408</v>
       </c>
       <c r="P7">
-        <v>0.9606704751589408</v>
+        <v>0.96067047515894077</v>
       </c>
       <c r="Q7">
         <v>1.0919997208629306</v>
@@ -889,7 +2166,7 @@
         <v>1.2380630097120604</v>
       </c>
       <c r="S7">
-        <v>1.400621515003608</v>
+        <v>1.4006215150036081</v>
       </c>
       <c r="T7">
         <v>1.5815212024126364</v>
@@ -898,13 +2175,13 @@
         <v>1.7826315713529446</v>
       </c>
       <c r="V7">
-        <v>2.005760899003269</v>
+        <v>2.0057608990032691</v>
       </c>
       <c r="W7">
         <v>2.2525512184209866</v>
       </c>
       <c r="X7">
-        <v>2.524362379079606</v>
+        <v>2.5243623790796059</v>
       </c>
       <c r="Y7">
         <v>2.8221606553925147</v>
@@ -913,32 +2190,32 @@
         <v>3.1464308987103604</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="C10">
         <v>1.9535148291666666</v>
       </c>
       <c r="D10">
-        <v>3.906029658333333</v>
+        <v>3.9060296583333329</v>
       </c>
       <c r="E10">
-        <v>5.8585444875</v>
+        <v>5.8585444874999997</v>
       </c>
       <c r="F10">
-        <v>7.811059316666666</v>
+        <v>7.8110593166666664</v>
       </c>
       <c r="G10">
-        <v>9.763574145833333</v>
+        <v>9.7635741458333332</v>
       </c>
       <c r="H10">
         <v>11.716088975</v>
@@ -950,16 +2227,16 @@
         <v>15.621118633333333</v>
       </c>
       <c r="K10">
-        <v>17.5736334625</v>
+        <v>17.573633462499998</v>
       </c>
       <c r="L10">
-        <v>19.52614829166667</v>
+        <v>19.526148291666669</v>
       </c>
       <c r="M10">
         <v>21.478663120833332</v>
       </c>
       <c r="N10">
-        <v>23.43117795</v>
+        <v>23.431177949999999</v>
       </c>
       <c r="O10">
         <v>25.383692779166665</v>
@@ -968,37 +2245,37 @@
         <v>27.336207608333336</v>
       </c>
       <c r="Q10">
-        <v>29.2887224375</v>
+        <v>29.288722437499999</v>
       </c>
       <c r="R10">
         <v>31.241237266666666</v>
       </c>
       <c r="S10">
-        <v>33.19375209583334</v>
+        <v>33.193752095833339</v>
       </c>
       <c r="T10">
-        <v>35.146266925</v>
+        <v>35.146266924999999</v>
       </c>
       <c r="U10">
         <v>37.098781754166666</v>
       </c>
       <c r="V10">
-        <v>39.05129658333333</v>
+        <v>39.051296583333333</v>
       </c>
       <c r="W10">
-        <v>41.0038114125</v>
+        <v>41.003811412499999</v>
       </c>
       <c r="X10">
         <v>42.956326241666666</v>
       </c>
       <c r="Y10">
-        <v>44.90884107083333</v>
+        <v>44.908841070833333</v>
       </c>
       <c r="Z10">
         <v>46.8613559</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1078,15 +2355,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.003411222923418046</v>
+        <v>3.4112229234180458E-3</v>
       </c>
       <c r="B12">
         <v>-11.605147306027055</v>
       </c>
       <c r="C12">
-        <v>-3.995872384326091</v>
+        <v>-3.9958723843260908</v>
       </c>
       <c r="D12">
         <v>-3.2701522824291094</v>
@@ -1101,7 +2378,7 @@
         <v>-2.2493880603440455</v>
       </c>
       <c r="H12">
-        <v>-2.029978412674971</v>
+        <v>-2.0299784126749709</v>
       </c>
       <c r="I12">
         <v>-1.8375213077314607</v>
@@ -1125,16 +2402,16 @@
         <v>-0.9594408140577052</v>
       </c>
       <c r="P12">
-        <v>-0.8366687826155881</v>
+        <v>-0.83666878261558808</v>
       </c>
       <c r="Q12">
-        <v>-0.7172786093240364</v>
+        <v>-0.71727860932403642</v>
       </c>
       <c r="R12">
-        <v>-0.6005647734164671</v>
+        <v>-0.60056477341646708</v>
       </c>
       <c r="S12">
-        <v>-0.4859578246460787</v>
+        <v>-0.48595782464607867</v>
       </c>
       <c r="T12">
         <v>-0.37300287865207166</v>
@@ -1146,10 +2423,10 @@
         <v>-0.15073076353464188</v>
       </c>
       <c r="W12">
-        <v>-0.04098867263558969</v>
+        <v>-4.0988672635589689E-2</v>
       </c>
       <c r="X12">
-        <v>0.06795452558527898</v>
+        <v>6.795452558527898E-2</v>
       </c>
       <c r="Y12">
         <v>0.17608249002031057</v>
@@ -1158,9 +2435,9 @@
         <v>0.28328966938607403</v>
       </c>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.003331667499583542</v>
+        <v>3.331667499583542E-3</v>
       </c>
       <c r="B13">
         <v>-11.420784302100849</v>
@@ -1169,7 +2446,7 @@
         <v>-3.81075619995043</v>
       </c>
       <c r="D13">
-        <v>-3.084210092434169</v>
+        <v>-3.0842100924341689</v>
       </c>
       <c r="E13">
         <v>-2.6441050288075134</v>
@@ -1178,7 +2455,7 @@
         <v>-2.3206075418297756</v>
       </c>
       <c r="G13">
-        <v>-2.060431696239898</v>
+        <v>-2.0604316962398981</v>
       </c>
       <c r="H13">
         <v>-1.8397975830962243</v>
@@ -1199,13 +2476,13 @@
         <v>-1.0200925759383102</v>
       </c>
       <c r="N13">
-        <v>-0.8853213697294672</v>
+        <v>-0.88532136972946718</v>
       </c>
       <c r="O13">
-        <v>-0.7555995125030412</v>
+        <v>-0.75559951250304125</v>
       </c>
       <c r="P13">
-        <v>-0.6297857794378303</v>
+        <v>-0.62978577943783032</v>
       </c>
       <c r="Q13">
         <v>-0.5069543520485047</v>
@@ -1214,16 +2491,16 @@
         <v>-0.38634330101520237</v>
       </c>
       <c r="S13">
-        <v>-0.2673214697985593</v>
+        <v>-0.26732146979855931</v>
       </c>
       <c r="T13">
         <v>-0.1493683775446672</v>
       </c>
       <c r="U13">
-        <v>-0.03206393163777815</v>
+        <v>-3.2063931637778147E-2</v>
       </c>
       <c r="V13">
-        <v>0.08491410457574017</v>
+        <v>8.4914104575740168E-2</v>
       </c>
       <c r="W13">
         <v>0.20178648706998767</v>
@@ -1235,30 +2512,30 @@
         <v>0.43553941556311576</v>
       </c>
       <c r="Z13">
-        <v>0.5522743030567119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26">
+        <v>0.55227430305671188</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.0032451728054518907</v>
+        <v>3.2451728054518907E-3</v>
       </c>
       <c r="B14">
         <v>-11.259033836456956</v>
       </c>
       <c r="C14">
-        <v>-3.643614442596813</v>
+        <v>-3.6436144425968129</v>
       </c>
       <c r="D14">
-        <v>-2.911363925376755</v>
+        <v>-2.9113639253767549</v>
       </c>
       <c r="E14">
         <v>-2.4652197242096325</v>
       </c>
       <c r="F14">
-        <v>-2.135326073486108</v>
+        <v>-2.1353260734861079</v>
       </c>
       <c r="G14">
-        <v>-1.868374478487823</v>
+        <v>-1.8683744784878229</v>
       </c>
       <c r="H14">
         <v>-1.6405628625405537</v>
@@ -1273,16 +2550,16 @@
         <v>-1.087574254052325</v>
       </c>
       <c r="L14">
-        <v>-0.9290242536844393</v>
+        <v>-0.92902425368443931</v>
       </c>
       <c r="M14">
         <v>-0.7783586496872219</v>
       </c>
       <c r="N14">
-        <v>-0.6337449144914354</v>
+        <v>-0.63374491449143544</v>
       </c>
       <c r="O14">
-        <v>-0.4937910366728759</v>
+        <v>-0.49379103667287588</v>
       </c>
       <c r="P14">
         <v>-0.35743015717027365</v>
@@ -1291,13 +2568,13 @@
         <v>-0.22385097986487862</v>
       </c>
       <c r="R14">
-        <v>-0.09245699840936435</v>
+        <v>-9.2456998409364347E-2</v>
       </c>
       <c r="S14">
-        <v>0.03715588808655996</v>
+        <v>3.7155888086559959E-2</v>
       </c>
       <c r="T14">
-        <v>0.1652108637445336</v>
+        <v>0.16521086374453359</v>
       </c>
       <c r="U14">
         <v>0.2917572538492102</v>
@@ -1306,33 +2583,33 @@
         <v>0.41667939072572685</v>
       </c>
       <c r="W14">
-        <v>0.5397130960313329</v>
+        <v>0.53971309603133288</v>
       </c>
       <c r="X14">
-        <v>0.6604740114942905</v>
+        <v>0.66047401149429052</v>
       </c>
       <c r="Y14">
-        <v>0.7784987839964441</v>
+        <v>0.77849878399644412</v>
       </c>
       <c r="Z14">
         <v>0.8932957105667424</v>
       </c>
     </row>
-    <row r="15" spans="1:26">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0.0030945381401825778</v>
+        <v>3.0945381401825778E-3</v>
       </c>
       <c r="B15">
         <v>-10.899159748986126</v>
       </c>
       <c r="C15">
-        <v>-3.285403499032817</v>
+        <v>-3.2854034990328169</v>
       </c>
       <c r="D15">
         <v>-2.5549501337033895</v>
       </c>
       <c r="E15">
-        <v>-2.110751576716211</v>
+        <v>-2.1107515767162108</v>
       </c>
       <c r="F15">
         <v>-1.7829682760180394</v>
@@ -1347,13 +2624,13 @@
         <v>-1.0942984860402398</v>
       </c>
       <c r="J15">
-        <v>-0.9145965075610273</v>
+        <v>-0.91459650756102728</v>
       </c>
       <c r="K15">
-        <v>-0.7489434534924628</v>
+        <v>-0.74894345349246283</v>
       </c>
       <c r="L15">
-        <v>-0.5939427046117786</v>
+        <v>-0.59394270461177856</v>
       </c>
       <c r="M15">
         <v>-0.44715790033829933</v>
@@ -1365,10 +2642,10 @@
         <v>-0.17145527692553925</v>
       </c>
       <c r="P15">
-        <v>-0.04012382667225934</v>
+        <v>-4.012382667225934E-2</v>
       </c>
       <c r="Q15">
-        <v>0.08801062170265372</v>
+        <v>8.8010621702653724E-2</v>
       </c>
       <c r="R15">
         <v>0.21354806934207468</v>
@@ -1377,19 +2654,19 @@
         <v>0.33691607739761303</v>
       </c>
       <c r="T15">
-        <v>0.4583871701944943</v>
+        <v>0.45838717019449432</v>
       </c>
       <c r="U15">
-        <v>0.5780906834030081</v>
+        <v>0.57809068340300807</v>
       </c>
       <c r="V15">
-        <v>0.6960234895160966</v>
+        <v>0.69602348951609661</v>
       </c>
       <c r="W15">
-        <v>0.8120634487195262</v>
+        <v>0.81206344871952618</v>
       </c>
       <c r="X15">
-        <v>0.9259885077011974</v>
+        <v>0.92598850770119745</v>
       </c>
       <c r="Y15">
         <v>1.0375027814319202</v>
@@ -1398,12 +2675,12 @@
         <v>1.1462687624248866</v>
       </c>
     </row>
-    <row r="17" spans="1:26">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1413,19 +2690,43 @@
       <c r="C18" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:26">
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="B19">
-        <v>-18378.57581055563</v>
+        <v>-18378.575810555631</v>
       </c>
       <c r="C19">
-        <v>579.513410356215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26">
+        <v>579.51341035621499</v>
+      </c>
+      <c r="D19">
+        <v>-23.623738341661344</v>
+      </c>
+      <c r="E19">
+        <v>1.8966067800595494</v>
+      </c>
+      <c r="F19">
+        <v>5.8350774600505563E-2</v>
+      </c>
+      <c r="G19">
+        <v>1.3310358084648701E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.9535148291666666</v>
       </c>
@@ -1435,52 +2736,112 @@
       <c r="C20">
         <v>496.3133063113973</v>
       </c>
-    </row>
-    <row r="21" spans="1:26">
+      <c r="D20">
+        <v>-24.356229144180258</v>
+      </c>
+      <c r="E20">
+        <v>1.6243130270365327</v>
+      </c>
+      <c r="F20">
+        <v>5.3430099052986631E-2</v>
+      </c>
+      <c r="G20">
+        <v>1.0438101644492711E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>3.906029658333333</v>
+        <v>3.9060296583333329</v>
       </c>
       <c r="B21">
         <v>-18657.396694606457</v>
       </c>
       <c r="C21">
-        <v>408.4859770731027</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26">
+        <v>408.48597707310267</v>
+      </c>
+      <c r="D21">
+        <v>-25.122544341889313</v>
+      </c>
+      <c r="E21">
+        <v>1.3368754886964236</v>
+      </c>
+      <c r="F21">
+        <v>4.8725753339353951E-2</v>
+      </c>
+      <c r="G21">
+        <v>7.8345731166590757E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>5.8585444875</v>
+        <v>5.8585444874999997</v>
       </c>
       <c r="B22">
         <v>-18808.527027553635</v>
       </c>
       <c r="C22">
-        <v>316.3657642400436</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26">
+        <v>316.36576424004357</v>
+      </c>
+      <c r="D22">
+        <v>-25.924735401642966</v>
+      </c>
+      <c r="E22">
+        <v>1.0353883839677958</v>
+      </c>
+      <c r="F22">
+        <v>4.4244288884486768E-2</v>
+      </c>
+      <c r="G22">
+        <v>5.5096793228578038E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>7.811059316666666</v>
+        <v>7.8110593166666664</v>
       </c>
       <c r="B23">
-        <v>-18968.09808718258</v>
+        <v>-18968.098087182581</v>
       </c>
       <c r="C23">
         <v>221.76317513179177</v>
       </c>
-    </row>
-    <row r="24" spans="1:26">
+      <c r="D23">
+        <v>-26.764901034589581</v>
+      </c>
+      <c r="E23">
+        <v>0.7257770640095399</v>
+      </c>
+      <c r="F23">
+        <v>3.9991926612959049E-2</v>
+      </c>
+      <c r="G23">
+        <v>3.4909319356210321E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>9.763574145833333</v>
+        <v>9.7635741458333332</v>
       </c>
       <c r="B24">
         <v>-19136.574086069995</v>
       </c>
       <c r="C24">
-        <v>133.8686920886433</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26">
+        <v>133.86869208864329</v>
+      </c>
+      <c r="D24">
+        <v>-27.645147515681504</v>
+      </c>
+      <c r="E24">
+        <v>0.43811974756021632</v>
+      </c>
+      <c r="F24">
+        <v>3.5974425447651698E-2</v>
+      </c>
+      <c r="G24">
+        <v>1.8956253602412309E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11.716088975</v>
       </c>
@@ -1490,8 +2851,20 @@
       <c r="C25">
         <v>103.96776402404235</v>
       </c>
-    </row>
-    <row r="26" spans="1:26">
+      <c r="D25">
+        <v>-28.567530498312387</v>
+      </c>
+      <c r="E25">
+        <v>0.34026126510933347</v>
+      </c>
+      <c r="F25">
+        <v>3.2196930058117072E-2</v>
+      </c>
+      <c r="G25">
+        <v>1.3176279282671166E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>13.668603804166668</v>
       </c>
@@ -1501,8 +2874,20 @@
       <c r="C26">
         <v>182.08245031137267</v>
       </c>
-    </row>
-    <row r="27" spans="1:26">
+      <c r="D26">
+        <v>-29.533971951452347</v>
+      </c>
+      <c r="E26">
+        <v>0.59591167972822701</v>
+      </c>
+      <c r="F26">
+        <v>2.8663797593103193E-2</v>
+      </c>
+      <c r="G26">
+        <v>2.0543831340106484E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>15.621118633333333</v>
       </c>
@@ -1510,32 +2895,68 @@
         <v>-19699.543131531842</v>
       </c>
       <c r="C27">
-        <v>301.9546067034061</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26">
+        <v>301.95460670340611</v>
+      </c>
+      <c r="D27">
+        <v>-30.54614408494443</v>
+      </c>
+      <c r="E27">
+        <v>0.98822416204635255</v>
+      </c>
+      <c r="F27">
+        <v>2.53784044127351E-2</v>
+      </c>
+      <c r="G27">
+        <v>3.0163768347567757E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>17.5736334625</v>
+        <v>17.573633462499998</v>
       </c>
       <c r="B28">
         <v>-19907.354784993036</v>
       </c>
       <c r="C28">
-        <v>438.2813891644411</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26">
+        <v>438.28138916444112</v>
+      </c>
+      <c r="D28">
+        <v>-31.605310131500403</v>
+      </c>
+      <c r="E28">
+        <v>1.4343886429690142</v>
+      </c>
+      <c r="F28">
+        <v>2.2342935757566185E-2</v>
+      </c>
+      <c r="G28">
+        <v>3.8545429540168701E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>19.52614829166667</v>
+        <v>19.526148291666669</v>
       </c>
       <c r="B29">
         <v>-20125.368576459005</v>
       </c>
       <c r="C29">
-        <v>586.6344216766888</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26">
+        <v>586.63442167668882</v>
+      </c>
+      <c r="D29">
+        <v>-32.71210982080224</v>
+      </c>
+      <c r="E29">
+        <v>1.9199121222827598</v>
+      </c>
+      <c r="F29">
+        <v>1.9558163946167436E-2</v>
+      </c>
+      <c r="G29">
+        <v>4.5162216458651729E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>21.478663120833332</v>
       </c>
@@ -1543,21 +2964,45 @@
         <v>-20353.296595538857</v>
       </c>
       <c r="C30">
-        <v>746.0290239284012</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26">
+        <v>746.02902392840122</v>
+      </c>
+      <c r="D30">
+        <v>-33.866275743502754</v>
+      </c>
+      <c r="E30">
+        <v>2.4415719802482032</v>
+      </c>
+      <c r="F30">
+        <v>1.7023224159527506E-2</v>
+      </c>
+      <c r="G30">
+        <v>4.9989312635358822E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>23.43117795</v>
+        <v>23.431177949999999</v>
       </c>
       <c r="B31">
         <v>-20590.473158167642</v>
       </c>
       <c r="C31">
-        <v>916.189265828536</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26">
+        <v>916.18926582853601</v>
+      </c>
+      <c r="D31">
+        <v>-35.06626638401891</v>
+      </c>
+      <c r="E31">
+        <v>2.9984651646285174</v>
+      </c>
+      <c r="F31">
+        <v>1.4735401125032743E-2</v>
+      </c>
+      <c r="G31">
+        <v>5.3140640579429719E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>25.383692779166665</v>
       </c>
@@ -1565,32 +3010,68 @@
         <v>-20835.72351460252</v>
       </c>
       <c r="C32">
-        <v>1096.890090251264</v>
-      </c>
-    </row>
-    <row r="33" spans="1:26">
+        <v>1096.8900902512639</v>
+      </c>
+      <c r="D32">
+        <v>-36.308803820153599</v>
+      </c>
+      <c r="E32">
+        <v>3.5898551180582992</v>
+      </c>
+      <c r="F32">
+        <v>1.2689944836964506E-2</v>
+      </c>
+      <c r="G32">
+        <v>5.4790147617469172E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>27.336207608333336</v>
       </c>
       <c r="B33">
-        <v>-21087.20505574941</v>
+        <v>-21087.205055749411</v>
       </c>
       <c r="C33">
         <v>1287.6808536382866</v>
       </c>
-    </row>
-    <row r="34" spans="1:26">
+      <c r="D33">
+        <v>-37.588311169961109</v>
+      </c>
+      <c r="E33">
+        <v>4.2142669935145367</v>
+      </c>
+      <c r="F33">
+        <v>1.087993832215455E-2</v>
+      </c>
+      <c r="G33">
+        <v>5.5146035370249816E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>29.2887224375</v>
+        <v>29.288722437499999</v>
       </c>
       <c r="B34">
-        <v>-21342.22451509101</v>
+        <v>-21342.224515091009</v>
       </c>
       <c r="C34">
         <v>1487.6929960566301</v>
       </c>
-    </row>
-    <row r="35" spans="1:26">
+      <c r="D34">
+        <v>-38.89625992847386</v>
+      </c>
+      <c r="E34">
+        <v>4.8688582050823435</v>
+      </c>
+      <c r="F34">
+        <v>9.2962444407995257E-3</v>
+      </c>
+      <c r="G34">
+        <v>5.4437788827405003E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31.241237266666666</v>
       </c>
@@ -1598,12 +3079,24 @@
         <v>-21597.042519102582</v>
       </c>
       <c r="C35">
-        <v>1695.466411969708</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26">
+        <v>1695.4664119697079</v>
+      </c>
+      <c r="D35">
+        <v>-40.220464057396264</v>
+      </c>
+      <c r="E35">
+        <v>5.5488501816177136</v>
+      </c>
+      <c r="F35">
+        <v>7.9275603955511476E-3</v>
+      </c>
+      <c r="G35">
+        <v>5.2906419766200032E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>33.19375209583334</v>
+        <v>33.193752095833339</v>
       </c>
       <c r="B36">
         <v>-21846.688900603258</v>
@@ -1611,19 +3104,43 @@
       <c r="C36">
         <v>1908.7901861427886</v>
       </c>
-    </row>
-    <row r="37" spans="1:26">
+      <c r="D36">
+        <v>-41.544399070941012</v>
+      </c>
+      <c r="E36">
+        <v>6.2470071340096585</v>
+      </c>
+      <c r="F36">
+        <v>6.7606062222738874E-3</v>
+      </c>
+      <c r="G36">
+        <v>5.0795291578514239E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35.146266925</v>
+        <v>35.146266924999999</v>
       </c>
       <c r="B37">
-        <v>-22084.82827389003</v>
+        <v>-22084.828273890031</v>
       </c>
       <c r="C37">
         <v>2124.5831469199175</v>
       </c>
-    </row>
-    <row r="38" spans="1:26">
+      <c r="D37">
+        <v>-42.846679969364715</v>
+      </c>
+      <c r="E37">
+        <v>6.9532451350378901</v>
+      </c>
+      <c r="F37">
+        <v>5.7804652545097365E-3</v>
+      </c>
+      <c r="G37">
+        <v>4.8341057931297572E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37.098781754166666</v>
       </c>
@@ -1633,21 +3150,45 @@
       <c r="C38">
         <v>2338.8626363207395</v>
       </c>
-    </row>
-    <row r="39" spans="1:26">
+      <c r="D38">
+        <v>-44.100893352603094</v>
+      </c>
+      <c r="E38">
+        <v>7.6545299114772982</v>
+      </c>
+      <c r="F38">
+        <v>4.9710792824347984E-3</v>
+      </c>
+      <c r="G38">
+        <v>4.5765164638113436E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>39.05129658333333</v>
+        <v>39.051296583333333</v>
       </c>
       <c r="B39">
-        <v>-22494.43337632375</v>
+        <v>-22494.433376323748</v>
       </c>
       <c r="C39">
         <v>2546.8655102217203</v>
       </c>
-    </row>
-    <row r="40" spans="1:26">
+      <c r="D39">
+        <v>-45.276025148907131</v>
+      </c>
+      <c r="E39">
+        <v>8.3352728483318241</v>
+      </c>
+      <c r="F39">
+        <v>4.3158794124439114E-3</v>
+      </c>
+      <c r="G39">
+        <v>4.32668160714016E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>41.0038114125</v>
+        <v>41.003811412499999</v>
       </c>
       <c r="B40">
         <v>-22647.113308360218</v>
@@ -1655,8 +3196,20 @@
       <c r="C40">
         <v>2743.3829540558895</v>
       </c>
-    </row>
-    <row r="41" spans="1:26">
+      <c r="D40">
+        <v>-46.337720616959189</v>
+      </c>
+      <c r="E40">
+        <v>8.9784267593806728</v>
+      </c>
+      <c r="F40">
+        <v>3.7985085128561329E-3</v>
+      </c>
+      <c r="G40">
+        <v>4.1018442253984077E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>42.956326241666666</v>
       </c>
@@ -1664,12 +3217,24 @@
         <v>-22751.789332432345</v>
       </c>
       <c r="C41">
-        <v>2923.336062016438</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26">
+        <v>2923.3360620164381</v>
+      </c>
+      <c r="D41">
+        <v>-47.250516866640211</v>
+      </c>
+      <c r="E41">
+        <v>9.5673696182542489</v>
+      </c>
+      <c r="F41">
+        <v>3.4035681542022257E-3</v>
+      </c>
+      <c r="G41">
+        <v>3.9164520965042013E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>44.90884107083333</v>
+        <v>44.908841070833333</v>
       </c>
       <c r="B42">
         <v>-22799.249974643626</v>
@@ -1677,8 +3242,20 @@
       <c r="C42">
         <v>3082.5454355357806</v>
       </c>
-    </row>
-    <row r="43" spans="1:26">
+      <c r="D42">
+        <v>-47.980978048356143</v>
+      </c>
+      <c r="E42">
+        <v>10.088423267522195</v>
+      </c>
+      <c r="F42">
+        <v>3.1173087574694648E-3</v>
+      </c>
+      <c r="G42">
+        <v>3.7824128443662256E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>46.8613559</v>
       </c>
@@ -1688,8 +3265,21 @@
       <c r="C43">
         <v>3218.5493269153303</v>
       </c>
+      <c r="D43">
+        <v>-48.501368268275641</v>
+      </c>
+      <c r="E43">
+        <v>10.533531004280835</v>
+      </c>
+      <c r="F43">
+        <v>2.9281812443090272E-3</v>
+      </c>
+      <c r="G43">
+        <v>3.7096910936540699E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>